<commit_message>
hanergy ceping result table creation in doing
</commit_message>
<xml_diff>
--- a/src/test/resources/hanergy-ceping.xlsx
+++ b/src/test/resources/hanergy-ceping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bingoo/GitHub/excel2javabeans/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB161C0E-DF6D-2C4B-A0C6-751AC0D87DD1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3E66F57-7222-EA40-9401-80ECB0699600}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{ED7C35D1-08C2-1B4F-A1CE-BB55E02E4662}"/>
+    <workbookView xWindow="20" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="1" xr2:uid="{ED7C35D1-08C2-1B4F-A1CE-BB55E02E4662}"/>
   </bookViews>
   <sheets>
     <sheet name="有评语-模板" sheetId="5" r:id="rId1"/>
@@ -769,7 +769,7 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -873,10 +873,208 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -888,206 +1086,11 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="10" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="10" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="10" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="10" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1098,11 +1101,20 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -4829,8 +4841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B0B56D7-DA51-554E-86D1-0655EAEF35DF}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="107" zoomScaleSheetLayoutView="125" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView zoomScale="150" zoomScaleNormal="107" zoomScaleSheetLayoutView="125" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="17"/>
@@ -4846,36 +4858,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="32.25" customHeight="1">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="91"/>
-      <c r="C1" s="91"/>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91"/>
-      <c r="F1" s="91"/>
-      <c r="G1" s="91"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A2" s="92" t="s">
+      <c r="A2" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="92"/>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="92"/>
-      <c r="F2" s="92"/>
-      <c r="G2" s="92"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
     </row>
     <row r="3" spans="1:7" s="8" customFormat="1" ht="27" customHeight="1">
       <c r="A3" s="34" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="34"/>
-      <c r="C3" s="92" t="s">
+      <c r="C3" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="92"/>
+      <c r="D3" s="47"/>
       <c r="E3" s="6"/>
       <c r="F3" s="34" t="s">
         <v>4</v>
@@ -4887,10 +4899,10 @@
         <v>5</v>
       </c>
       <c r="B4" s="34"/>
-      <c r="C4" s="92" t="s">
+      <c r="C4" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="92"/>
+      <c r="D4" s="47"/>
       <c r="E4" s="10"/>
       <c r="F4" s="32" t="s">
         <v>7</v>
@@ -4898,65 +4910,65 @@
       <c r="G4" s="34"/>
     </row>
     <row r="5" spans="1:7" s="8" customFormat="1" ht="49.5" customHeight="1">
-      <c r="A5" s="93" t="s">
+      <c r="A5" s="112" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="87" t="s">
+      <c r="B5" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="96">
+      <c r="C5" s="52">
         <v>1.2</v>
       </c>
-      <c r="D5" s="97"/>
-      <c r="E5" s="97"/>
-      <c r="F5" s="97"/>
-      <c r="G5" s="98"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="54"/>
     </row>
     <row r="6" spans="1:7" s="13" customFormat="1" ht="48" customHeight="1">
-      <c r="A6" s="94"/>
-      <c r="B6" s="95"/>
-      <c r="C6" s="99"/>
-      <c r="D6" s="100"/>
-      <c r="E6" s="100"/>
-      <c r="F6" s="100"/>
-      <c r="G6" s="101"/>
-    </row>
-    <row r="7" spans="1:7" s="111" customFormat="1" ht="40" customHeight="1">
-      <c r="A7" s="94"/>
-      <c r="B7" s="35" t="s">
+      <c r="A6" s="112"/>
+      <c r="B6" s="51"/>
+      <c r="C6" s="55"/>
+      <c r="D6" s="56"/>
+      <c r="E6" s="56"/>
+      <c r="F6" s="56"/>
+      <c r="G6" s="57"/>
+    </row>
+    <row r="7" spans="1:7" s="37" customFormat="1" ht="40" customHeight="1">
+      <c r="A7" s="112"/>
+      <c r="B7" s="111" t="s">
         <v>90</v>
       </c>
-      <c r="C7" s="36" t="s">
+      <c r="C7" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="D7" s="90"/>
-      <c r="E7" s="90"/>
-      <c r="F7" s="90"/>
-      <c r="G7" s="90"/>
+      <c r="D7" s="113"/>
+      <c r="E7" s="113"/>
+      <c r="F7" s="113"/>
+      <c r="G7" s="113"/>
     </row>
     <row r="8" spans="1:7" s="8" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A8" s="75" t="s">
+      <c r="A8" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="89"/>
-      <c r="C8" s="89"/>
-      <c r="D8" s="89"/>
-      <c r="E8" s="89"/>
-      <c r="F8" s="89"/>
-      <c r="G8" s="76"/>
+      <c r="B8" s="45"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="39"/>
     </row>
     <row r="9" spans="1:7" s="8" customFormat="1" ht="18" customHeight="1">
       <c r="A9" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="75" t="s">
+      <c r="B9" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="76"/>
-      <c r="D9" s="77" t="s">
+      <c r="C9" s="39"/>
+      <c r="D9" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="77"/>
+      <c r="E9" s="40"/>
       <c r="F9" s="33" t="s">
         <v>14</v>
       </c>
@@ -4968,35 +4980,32 @@
       <c r="A10" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="81" t="s">
+      <c r="B10" s="114" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="82"/>
-      <c r="D10" s="64" t="s">
+      <c r="C10" s="115"/>
+      <c r="D10" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="65"/>
-      <c r="F10" s="36"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="35"/>
       <c r="G10" s="18" t="s">
         <v>19</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="A8:G8"/>
+  <mergeCells count="11">
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A2:G2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:A7"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="C5:G5"/>
     <mergeCell ref="C6:G6"/>
-    <mergeCell ref="D7:G7"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="A8:G8"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <printOptions horizontalCentered="1" gridLines="1"/>
@@ -5013,8 +5022,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{406DFA14-B27B-0342-9479-E669BC030586}">
   <dimension ref="A1:Q10"/>
   <sheetViews>
-    <sheetView zoomScale="135" zoomScaleNormal="100" zoomScaleSheetLayoutView="125" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" zoomScale="135" zoomScaleNormal="100" zoomScaleSheetLayoutView="125" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="17"/>
@@ -5035,15 +5044,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="1" customFormat="1" ht="32.25" customHeight="1">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="91"/>
-      <c r="C1" s="91"/>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91"/>
-      <c r="F1" s="91"/>
-      <c r="G1" s="91"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
       <c r="J1" s="2"/>
       <c r="L1" s="3"/>
       <c r="M1" s="4"/>
@@ -5052,15 +5061,15 @@
       <c r="P1" s="4"/>
     </row>
     <row r="2" spans="1:17" s="1" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A2" s="92" t="s">
+      <c r="A2" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="92"/>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="92"/>
-      <c r="F2" s="92"/>
-      <c r="G2" s="92"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
       <c r="J2" s="2"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
@@ -5073,10 +5082,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="34"/>
-      <c r="C3" s="92" t="s">
+      <c r="C3" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="92"/>
+      <c r="D3" s="47"/>
       <c r="E3" s="6"/>
       <c r="F3" s="34" t="s">
         <v>4</v>
@@ -5094,10 +5103,10 @@
         <v>5</v>
       </c>
       <c r="B4" s="34"/>
-      <c r="C4" s="92" t="s">
+      <c r="C4" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="92"/>
+      <c r="D4" s="47"/>
       <c r="E4" s="10"/>
       <c r="F4" s="32" t="s">
         <v>7</v>
@@ -5111,19 +5120,19 @@
       <c r="Q4" s="4"/>
     </row>
     <row r="5" spans="1:17" s="8" customFormat="1" ht="49.5" customHeight="1">
-      <c r="A5" s="93" t="s">
+      <c r="A5" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="87" t="s">
+      <c r="B5" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="96">
+      <c r="C5" s="52">
         <v>6</v>
       </c>
-      <c r="D5" s="97"/>
-      <c r="E5" s="97"/>
-      <c r="F5" s="97"/>
-      <c r="G5" s="98"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="54"/>
       <c r="H5" s="31"/>
       <c r="J5" s="12"/>
       <c r="K5" s="4"/>
@@ -5135,28 +5144,28 @@
       <c r="Q5" s="4"/>
     </row>
     <row r="6" spans="1:17" s="13" customFormat="1" ht="48" customHeight="1">
-      <c r="A6" s="94"/>
-      <c r="B6" s="95"/>
-      <c r="C6" s="104"/>
-      <c r="D6" s="105"/>
-      <c r="E6" s="105"/>
-      <c r="F6" s="105"/>
-      <c r="G6" s="106"/>
+      <c r="A6" s="49"/>
+      <c r="B6" s="51"/>
+      <c r="C6" s="59"/>
+      <c r="D6" s="60"/>
+      <c r="E6" s="60"/>
+      <c r="F6" s="60"/>
+      <c r="G6" s="61"/>
       <c r="I6" s="14"/>
       <c r="J6" s="14"/>
       <c r="K6" s="14"/>
       <c r="L6" s="14"/>
     </row>
     <row r="7" spans="1:17" s="8" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A7" s="75" t="s">
+      <c r="A7" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="89"/>
-      <c r="C7" s="89"/>
-      <c r="D7" s="89"/>
-      <c r="E7" s="89"/>
-      <c r="F7" s="89"/>
-      <c r="G7" s="76"/>
+      <c r="B7" s="45"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="39"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
@@ -5166,14 +5175,14 @@
       <c r="A8" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="75" t="s">
+      <c r="B8" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="76"/>
-      <c r="D8" s="77" t="s">
+      <c r="C8" s="39"/>
+      <c r="D8" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="77"/>
+      <c r="E8" s="40"/>
       <c r="F8" s="33" t="s">
         <v>14</v>
       </c>
@@ -5186,18 +5195,18 @@
       <c r="L8" s="4"/>
     </row>
     <row r="9" spans="1:17" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A9" s="110" t="s">
+      <c r="A9" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="81" t="s">
+      <c r="B9" s="114" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="82"/>
-      <c r="D9" s="64" t="s">
+      <c r="C9" s="115"/>
+      <c r="D9" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="65"/>
-      <c r="F9" s="36"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="35"/>
       <c r="G9" s="18" t="s">
         <v>19</v>
       </c>
@@ -5217,12 +5226,7 @@
       <c r="P10" s="28"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="A7:G7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:E9"/>
+  <mergeCells count="12">
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A2:G2"/>
     <mergeCell ref="C3:D3"/>
@@ -5231,6 +5235,10 @@
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="C5:G5"/>
     <mergeCell ref="C6:G6"/>
+    <mergeCell ref="A7:G7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="H5">
@@ -5254,8 +5262,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3B0BF8C-2422-9C41-8C7B-F10DC2F2FA45}">
   <dimension ref="A1:I75"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="177" zoomScaleNormal="107" zoomScaleSheetLayoutView="125" workbookViewId="0">
-      <selection activeCell="M49" sqref="M49"/>
+    <sheetView topLeftCell="A15" zoomScale="177" zoomScaleNormal="107" zoomScaleSheetLayoutView="125" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22:C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="17"/>
@@ -5271,36 +5279,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="32.25" customHeight="1">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="91"/>
-      <c r="C1" s="91"/>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91"/>
-      <c r="F1" s="91"/>
-      <c r="G1" s="91"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A2" s="92" t="s">
+      <c r="A2" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="92"/>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="92"/>
-      <c r="F2" s="92"/>
-      <c r="G2" s="92"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
     </row>
     <row r="3" spans="1:7" s="8" customFormat="1" ht="27" customHeight="1">
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="5"/>
-      <c r="C3" s="92" t="s">
+      <c r="C3" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="92"/>
+      <c r="D3" s="47"/>
       <c r="E3" s="6"/>
       <c r="F3" s="5" t="s">
         <v>4</v>
@@ -5312,10 +5320,10 @@
         <v>5</v>
       </c>
       <c r="B4" s="5"/>
-      <c r="C4" s="92" t="s">
+      <c r="C4" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="92"/>
+      <c r="D4" s="47"/>
       <c r="E4" s="10"/>
       <c r="F4" s="25" t="s">
         <v>7</v>
@@ -5323,186 +5331,186 @@
       <c r="G4" s="5"/>
     </row>
     <row r="5" spans="1:7" s="8" customFormat="1" ht="49.5" customHeight="1">
-      <c r="A5" s="93" t="s">
+      <c r="A5" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="87" t="s">
+      <c r="B5" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="96">
+      <c r="C5" s="52">
         <v>1.2</v>
       </c>
-      <c r="D5" s="97"/>
-      <c r="E5" s="97"/>
-      <c r="F5" s="97"/>
-      <c r="G5" s="98"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="54"/>
     </row>
     <row r="6" spans="1:7" s="13" customFormat="1" ht="48" customHeight="1">
-      <c r="A6" s="94"/>
-      <c r="B6" s="95"/>
-      <c r="C6" s="99"/>
-      <c r="D6" s="100"/>
-      <c r="E6" s="100"/>
-      <c r="F6" s="100"/>
-      <c r="G6" s="101"/>
+      <c r="A6" s="49"/>
+      <c r="B6" s="51"/>
+      <c r="C6" s="55"/>
+      <c r="D6" s="56"/>
+      <c r="E6" s="56"/>
+      <c r="F6" s="56"/>
+      <c r="G6" s="57"/>
     </row>
     <row r="7" spans="1:7" s="13" customFormat="1" ht="40" customHeight="1">
-      <c r="A7" s="94"/>
-      <c r="B7" s="102" t="s">
+      <c r="A7" s="49"/>
+      <c r="B7" s="62" t="s">
         <v>90</v>
       </c>
       <c r="C7" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="D7" s="86"/>
-      <c r="E7" s="86"/>
-      <c r="F7" s="86"/>
-      <c r="G7" s="86"/>
+      <c r="D7" s="64"/>
+      <c r="E7" s="64"/>
+      <c r="F7" s="64"/>
+      <c r="G7" s="64"/>
     </row>
     <row r="8" spans="1:7" s="13" customFormat="1" ht="40" customHeight="1">
-      <c r="A8" s="94"/>
-      <c r="B8" s="103"/>
-      <c r="C8" s="90" t="s">
+      <c r="A8" s="49"/>
+      <c r="B8" s="63"/>
+      <c r="C8" s="58" t="s">
         <v>91</v>
       </c>
-      <c r="D8" s="86"/>
-      <c r="E8" s="86"/>
-      <c r="F8" s="86"/>
-      <c r="G8" s="86"/>
+      <c r="D8" s="64"/>
+      <c r="E8" s="64"/>
+      <c r="F8" s="64"/>
+      <c r="G8" s="64"/>
     </row>
     <row r="9" spans="1:7" s="13" customFormat="1" ht="40" customHeight="1">
-      <c r="A9" s="94"/>
-      <c r="B9" s="103"/>
-      <c r="C9" s="90"/>
-      <c r="D9" s="86"/>
-      <c r="E9" s="86"/>
-      <c r="F9" s="86"/>
-      <c r="G9" s="86"/>
+      <c r="A9" s="49"/>
+      <c r="B9" s="63"/>
+      <c r="C9" s="58"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="64"/>
+      <c r="F9" s="64"/>
+      <c r="G9" s="64"/>
     </row>
     <row r="10" spans="1:7" s="13" customFormat="1" ht="40" customHeight="1">
-      <c r="A10" s="94"/>
-      <c r="B10" s="103"/>
-      <c r="C10" s="90"/>
-      <c r="D10" s="86"/>
-      <c r="E10" s="86"/>
-      <c r="F10" s="86"/>
-      <c r="G10" s="86"/>
+      <c r="A10" s="49"/>
+      <c r="B10" s="63"/>
+      <c r="C10" s="58"/>
+      <c r="D10" s="64"/>
+      <c r="E10" s="64"/>
+      <c r="F10" s="64"/>
+      <c r="G10" s="64"/>
     </row>
     <row r="11" spans="1:7" s="13" customFormat="1" ht="40" customHeight="1">
-      <c r="A11" s="94"/>
-      <c r="B11" s="103"/>
-      <c r="C11" s="90"/>
-      <c r="D11" s="83"/>
-      <c r="E11" s="84"/>
-      <c r="F11" s="84"/>
-      <c r="G11" s="85"/>
+      <c r="A11" s="49"/>
+      <c r="B11" s="63"/>
+      <c r="C11" s="58"/>
+      <c r="D11" s="65"/>
+      <c r="E11" s="66"/>
+      <c r="F11" s="66"/>
+      <c r="G11" s="67"/>
     </row>
     <row r="12" spans="1:7" s="13" customFormat="1" ht="40" customHeight="1">
-      <c r="A12" s="94"/>
-      <c r="B12" s="103"/>
-      <c r="C12" s="90"/>
-      <c r="D12" s="86"/>
-      <c r="E12" s="86"/>
-      <c r="F12" s="86"/>
-      <c r="G12" s="86"/>
+      <c r="A12" s="49"/>
+      <c r="B12" s="63"/>
+      <c r="C12" s="58"/>
+      <c r="D12" s="64"/>
+      <c r="E12" s="64"/>
+      <c r="F12" s="64"/>
+      <c r="G12" s="64"/>
     </row>
     <row r="13" spans="1:7" s="13" customFormat="1" ht="40" customHeight="1">
-      <c r="A13" s="94"/>
-      <c r="B13" s="103"/>
-      <c r="C13" s="90"/>
-      <c r="D13" s="86"/>
-      <c r="E13" s="86"/>
-      <c r="F13" s="86"/>
-      <c r="G13" s="86"/>
+      <c r="A13" s="49"/>
+      <c r="B13" s="63"/>
+      <c r="C13" s="58"/>
+      <c r="D13" s="64"/>
+      <c r="E13" s="64"/>
+      <c r="F13" s="64"/>
+      <c r="G13" s="64"/>
     </row>
     <row r="14" spans="1:7" s="13" customFormat="1" ht="40" customHeight="1">
-      <c r="A14" s="94"/>
-      <c r="B14" s="103"/>
-      <c r="C14" s="90"/>
-      <c r="D14" s="83"/>
-      <c r="E14" s="84"/>
-      <c r="F14" s="84"/>
-      <c r="G14" s="85"/>
+      <c r="A14" s="49"/>
+      <c r="B14" s="63"/>
+      <c r="C14" s="58"/>
+      <c r="D14" s="65"/>
+      <c r="E14" s="66"/>
+      <c r="F14" s="66"/>
+      <c r="G14" s="67"/>
     </row>
     <row r="15" spans="1:7" s="13" customFormat="1" ht="40" customHeight="1">
-      <c r="A15" s="94"/>
-      <c r="B15" s="103"/>
-      <c r="C15" s="90"/>
-      <c r="D15" s="83"/>
-      <c r="E15" s="84"/>
-      <c r="F15" s="84"/>
-      <c r="G15" s="85"/>
+      <c r="A15" s="49"/>
+      <c r="B15" s="63"/>
+      <c r="C15" s="58"/>
+      <c r="D15" s="65"/>
+      <c r="E15" s="66"/>
+      <c r="F15" s="66"/>
+      <c r="G15" s="67"/>
     </row>
     <row r="16" spans="1:7" s="13" customFormat="1" ht="40" customHeight="1">
-      <c r="A16" s="94"/>
-      <c r="B16" s="103"/>
-      <c r="C16" s="90"/>
-      <c r="D16" s="83"/>
-      <c r="E16" s="84"/>
-      <c r="F16" s="84"/>
-      <c r="G16" s="85"/>
+      <c r="A16" s="49"/>
+      <c r="B16" s="63"/>
+      <c r="C16" s="58"/>
+      <c r="D16" s="65"/>
+      <c r="E16" s="66"/>
+      <c r="F16" s="66"/>
+      <c r="G16" s="67"/>
     </row>
     <row r="17" spans="1:7" s="13" customFormat="1" ht="40" customHeight="1">
-      <c r="A17" s="94"/>
-      <c r="B17" s="103"/>
-      <c r="C17" s="90"/>
-      <c r="D17" s="83"/>
-      <c r="E17" s="84"/>
-      <c r="F17" s="84"/>
-      <c r="G17" s="85"/>
+      <c r="A17" s="49"/>
+      <c r="B17" s="63"/>
+      <c r="C17" s="58"/>
+      <c r="D17" s="65"/>
+      <c r="E17" s="66"/>
+      <c r="F17" s="66"/>
+      <c r="G17" s="67"/>
     </row>
     <row r="18" spans="1:7" s="13" customFormat="1" ht="40" customHeight="1">
-      <c r="A18" s="94"/>
-      <c r="B18" s="103"/>
-      <c r="C18" s="90"/>
-      <c r="D18" s="86"/>
-      <c r="E18" s="86"/>
-      <c r="F18" s="86"/>
-      <c r="G18" s="86"/>
+      <c r="A18" s="49"/>
+      <c r="B18" s="63"/>
+      <c r="C18" s="58"/>
+      <c r="D18" s="64"/>
+      <c r="E18" s="64"/>
+      <c r="F18" s="64"/>
+      <c r="G18" s="64"/>
     </row>
     <row r="19" spans="1:7" s="13" customFormat="1" ht="40" customHeight="1">
-      <c r="A19" s="94"/>
-      <c r="B19" s="103"/>
-      <c r="C19" s="87" t="s">
+      <c r="A19" s="49"/>
+      <c r="B19" s="63"/>
+      <c r="C19" s="50" t="s">
         <v>92</v>
       </c>
-      <c r="D19" s="86"/>
-      <c r="E19" s="86"/>
-      <c r="F19" s="86"/>
-      <c r="G19" s="86"/>
+      <c r="D19" s="64"/>
+      <c r="E19" s="64"/>
+      <c r="F19" s="64"/>
+      <c r="G19" s="64"/>
     </row>
     <row r="20" spans="1:7" s="13" customFormat="1" ht="40" customHeight="1">
-      <c r="A20" s="94"/>
-      <c r="B20" s="103"/>
-      <c r="C20" s="88"/>
-      <c r="D20" s="86"/>
-      <c r="E20" s="86"/>
-      <c r="F20" s="86"/>
-      <c r="G20" s="86"/>
+      <c r="A20" s="49"/>
+      <c r="B20" s="63"/>
+      <c r="C20" s="68"/>
+      <c r="D20" s="64"/>
+      <c r="E20" s="64"/>
+      <c r="F20" s="64"/>
+      <c r="G20" s="64"/>
     </row>
     <row r="21" spans="1:7" s="8" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A21" s="75" t="s">
+      <c r="A21" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="89"/>
-      <c r="C21" s="89"/>
-      <c r="D21" s="89"/>
-      <c r="E21" s="89"/>
-      <c r="F21" s="89"/>
-      <c r="G21" s="76"/>
+      <c r="B21" s="45"/>
+      <c r="C21" s="45"/>
+      <c r="D21" s="45"/>
+      <c r="E21" s="45"/>
+      <c r="F21" s="45"/>
+      <c r="G21" s="39"/>
     </row>
     <row r="22" spans="1:7" s="8" customFormat="1" ht="18" customHeight="1">
       <c r="A22" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="75" t="s">
+      <c r="B22" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="76"/>
-      <c r="D22" s="77" t="s">
+      <c r="C22" s="39"/>
+      <c r="D22" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="E22" s="77"/>
+      <c r="E22" s="40"/>
       <c r="F22" s="16" t="s">
         <v>14</v>
       </c>
@@ -5511,548 +5519,548 @@
       </c>
     </row>
     <row r="23" spans="1:7" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A23" s="78" t="s">
+      <c r="A23" s="69" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="81" t="s">
+      <c r="B23" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="C23" s="82"/>
-      <c r="D23" s="64" t="s">
+      <c r="C23" s="42"/>
+      <c r="D23" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="E23" s="65"/>
+      <c r="E23" s="44"/>
       <c r="F23" s="17"/>
       <c r="G23" s="18" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:7" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A24" s="79"/>
-      <c r="B24" s="69" t="s">
+      <c r="A24" s="70"/>
+      <c r="B24" s="72" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="70"/>
-      <c r="D24" s="64" t="s">
+      <c r="C24" s="73"/>
+      <c r="D24" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="E24" s="65"/>
-      <c r="F24" s="66">
+      <c r="E24" s="44"/>
+      <c r="F24" s="78">
         <v>2</v>
       </c>
-      <c r="G24" s="40" t="s">
+      <c r="G24" s="81" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:7" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A25" s="79"/>
-      <c r="B25" s="71"/>
-      <c r="C25" s="72"/>
-      <c r="D25" s="64" t="s">
+      <c r="A25" s="70"/>
+      <c r="B25" s="74"/>
+      <c r="C25" s="75"/>
+      <c r="D25" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="E25" s="65"/>
-      <c r="F25" s="67"/>
-      <c r="G25" s="41"/>
+      <c r="E25" s="44"/>
+      <c r="F25" s="79"/>
+      <c r="G25" s="82"/>
     </row>
     <row r="26" spans="1:7" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A26" s="79"/>
-      <c r="B26" s="71"/>
-      <c r="C26" s="72"/>
-      <c r="D26" s="64" t="s">
+      <c r="A26" s="70"/>
+      <c r="B26" s="74"/>
+      <c r="C26" s="75"/>
+      <c r="D26" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="E26" s="65"/>
-      <c r="F26" s="67"/>
-      <c r="G26" s="41"/>
+      <c r="E26" s="44"/>
+      <c r="F26" s="79"/>
+      <c r="G26" s="82"/>
     </row>
     <row r="27" spans="1:7" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A27" s="79"/>
-      <c r="B27" s="71"/>
-      <c r="C27" s="72"/>
-      <c r="D27" s="64" t="s">
+      <c r="A27" s="70"/>
+      <c r="B27" s="74"/>
+      <c r="C27" s="75"/>
+      <c r="D27" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="E27" s="65"/>
-      <c r="F27" s="67"/>
-      <c r="G27" s="41"/>
+      <c r="E27" s="44"/>
+      <c r="F27" s="79"/>
+      <c r="G27" s="82"/>
     </row>
     <row r="28" spans="1:7" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A28" s="79"/>
-      <c r="B28" s="73"/>
-      <c r="C28" s="74"/>
-      <c r="D28" s="64" t="s">
+      <c r="A28" s="70"/>
+      <c r="B28" s="76"/>
+      <c r="C28" s="77"/>
+      <c r="D28" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="E28" s="65"/>
-      <c r="F28" s="68"/>
-      <c r="G28" s="41"/>
+      <c r="E28" s="44"/>
+      <c r="F28" s="80"/>
+      <c r="G28" s="82"/>
     </row>
     <row r="29" spans="1:7" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A29" s="79"/>
-      <c r="B29" s="58" t="s">
+      <c r="A29" s="70"/>
+      <c r="B29" s="84" t="s">
         <v>27</v>
       </c>
-      <c r="C29" s="59"/>
-      <c r="D29" s="64" t="s">
+      <c r="C29" s="85"/>
+      <c r="D29" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="E29" s="65"/>
-      <c r="F29" s="66">
+      <c r="E29" s="44"/>
+      <c r="F29" s="78">
         <v>2</v>
       </c>
-      <c r="G29" s="41"/>
+      <c r="G29" s="82"/>
     </row>
     <row r="30" spans="1:7" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A30" s="79"/>
-      <c r="B30" s="60"/>
-      <c r="C30" s="61"/>
-      <c r="D30" s="64" t="s">
+      <c r="A30" s="70"/>
+      <c r="B30" s="88"/>
+      <c r="C30" s="89"/>
+      <c r="D30" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="E30" s="65"/>
-      <c r="F30" s="67"/>
-      <c r="G30" s="41"/>
+      <c r="E30" s="44"/>
+      <c r="F30" s="79"/>
+      <c r="G30" s="82"/>
     </row>
     <row r="31" spans="1:7" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A31" s="79"/>
-      <c r="B31" s="60"/>
-      <c r="C31" s="61"/>
-      <c r="D31" s="64" t="s">
+      <c r="A31" s="70"/>
+      <c r="B31" s="88"/>
+      <c r="C31" s="89"/>
+      <c r="D31" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="E31" s="65"/>
-      <c r="F31" s="67"/>
-      <c r="G31" s="41"/>
+      <c r="E31" s="44"/>
+      <c r="F31" s="79"/>
+      <c r="G31" s="82"/>
     </row>
     <row r="32" spans="1:7" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A32" s="79"/>
-      <c r="B32" s="60"/>
-      <c r="C32" s="61"/>
-      <c r="D32" s="64" t="s">
+      <c r="A32" s="70"/>
+      <c r="B32" s="88"/>
+      <c r="C32" s="89"/>
+      <c r="D32" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="E32" s="65"/>
-      <c r="F32" s="67"/>
-      <c r="G32" s="41"/>
+      <c r="E32" s="44"/>
+      <c r="F32" s="79"/>
+      <c r="G32" s="82"/>
     </row>
     <row r="33" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A33" s="79"/>
-      <c r="B33" s="62"/>
-      <c r="C33" s="63"/>
-      <c r="D33" s="64" t="s">
+      <c r="A33" s="70"/>
+      <c r="B33" s="86"/>
+      <c r="C33" s="87"/>
+      <c r="D33" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="E33" s="65"/>
-      <c r="F33" s="68"/>
-      <c r="G33" s="42"/>
+      <c r="E33" s="44"/>
+      <c r="F33" s="80"/>
+      <c r="G33" s="83"/>
     </row>
     <row r="34" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A34" s="79"/>
-      <c r="B34" s="58" t="s">
+      <c r="A34" s="70"/>
+      <c r="B34" s="84" t="s">
         <v>33</v>
       </c>
-      <c r="C34" s="59"/>
-      <c r="D34" s="64" t="s">
+      <c r="C34" s="85"/>
+      <c r="D34" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="E34" s="65"/>
-      <c r="F34" s="66">
+      <c r="E34" s="44"/>
+      <c r="F34" s="78">
         <v>0</v>
       </c>
-      <c r="G34" s="40" t="s">
+      <c r="G34" s="81" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="35" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A35" s="79"/>
-      <c r="B35" s="62"/>
-      <c r="C35" s="63"/>
-      <c r="D35" s="64" t="s">
+      <c r="A35" s="70"/>
+      <c r="B35" s="86"/>
+      <c r="C35" s="87"/>
+      <c r="D35" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="E35" s="65"/>
-      <c r="F35" s="68"/>
-      <c r="G35" s="42"/>
+      <c r="E35" s="44"/>
+      <c r="F35" s="80"/>
+      <c r="G35" s="83"/>
     </row>
     <row r="36" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A36" s="79"/>
-      <c r="B36" s="69" t="s">
+      <c r="A36" s="70"/>
+      <c r="B36" s="72" t="s">
         <v>36</v>
       </c>
-      <c r="C36" s="70"/>
-      <c r="D36" s="64" t="s">
+      <c r="C36" s="73"/>
+      <c r="D36" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="E36" s="65"/>
-      <c r="F36" s="66">
+      <c r="E36" s="44"/>
+      <c r="F36" s="78">
         <v>2</v>
       </c>
-      <c r="G36" s="40" t="s">
+      <c r="G36" s="81" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="37" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A37" s="79"/>
-      <c r="B37" s="71"/>
-      <c r="C37" s="72"/>
-      <c r="D37" s="64" t="s">
+      <c r="A37" s="70"/>
+      <c r="B37" s="74"/>
+      <c r="C37" s="75"/>
+      <c r="D37" s="43" t="s">
         <v>38</v>
       </c>
-      <c r="E37" s="65"/>
-      <c r="F37" s="67"/>
-      <c r="G37" s="41"/>
+      <c r="E37" s="44"/>
+      <c r="F37" s="79"/>
+      <c r="G37" s="82"/>
     </row>
     <row r="38" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A38" s="79"/>
-      <c r="B38" s="71"/>
-      <c r="C38" s="72"/>
-      <c r="D38" s="64" t="s">
+      <c r="A38" s="70"/>
+      <c r="B38" s="74"/>
+      <c r="C38" s="75"/>
+      <c r="D38" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="E38" s="65"/>
-      <c r="F38" s="67"/>
-      <c r="G38" s="41"/>
+      <c r="E38" s="44"/>
+      <c r="F38" s="79"/>
+      <c r="G38" s="82"/>
     </row>
     <row r="39" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A39" s="79"/>
-      <c r="B39" s="71"/>
-      <c r="C39" s="72"/>
-      <c r="D39" s="64" t="s">
+      <c r="A39" s="70"/>
+      <c r="B39" s="74"/>
+      <c r="C39" s="75"/>
+      <c r="D39" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="E39" s="65"/>
-      <c r="F39" s="67"/>
-      <c r="G39" s="41"/>
+      <c r="E39" s="44"/>
+      <c r="F39" s="79"/>
+      <c r="G39" s="82"/>
     </row>
     <row r="40" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A40" s="79"/>
-      <c r="B40" s="73"/>
-      <c r="C40" s="74"/>
-      <c r="D40" s="64" t="s">
+      <c r="A40" s="70"/>
+      <c r="B40" s="76"/>
+      <c r="C40" s="77"/>
+      <c r="D40" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="E40" s="65"/>
-      <c r="F40" s="68"/>
-      <c r="G40" s="41"/>
+      <c r="E40" s="44"/>
+      <c r="F40" s="80"/>
+      <c r="G40" s="82"/>
       <c r="I40" s="4"/>
     </row>
     <row r="41" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A41" s="79"/>
-      <c r="B41" s="58" t="s">
+      <c r="A41" s="70"/>
+      <c r="B41" s="84" t="s">
         <v>42</v>
       </c>
-      <c r="C41" s="59"/>
-      <c r="D41" s="64" t="s">
+      <c r="C41" s="85"/>
+      <c r="D41" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="E41" s="65"/>
-      <c r="F41" s="66">
+      <c r="E41" s="44"/>
+      <c r="F41" s="78">
         <v>2</v>
       </c>
-      <c r="G41" s="41"/>
+      <c r="G41" s="82"/>
     </row>
     <row r="42" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A42" s="79"/>
-      <c r="B42" s="60"/>
-      <c r="C42" s="61"/>
-      <c r="D42" s="64" t="s">
+      <c r="A42" s="70"/>
+      <c r="B42" s="88"/>
+      <c r="C42" s="89"/>
+      <c r="D42" s="43" t="s">
         <v>44</v>
       </c>
-      <c r="E42" s="65"/>
-      <c r="F42" s="67"/>
-      <c r="G42" s="41"/>
+      <c r="E42" s="44"/>
+      <c r="F42" s="79"/>
+      <c r="G42" s="82"/>
     </row>
     <row r="43" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A43" s="79"/>
-      <c r="B43" s="60"/>
-      <c r="C43" s="61"/>
-      <c r="D43" s="64" t="s">
+      <c r="A43" s="70"/>
+      <c r="B43" s="88"/>
+      <c r="C43" s="89"/>
+      <c r="D43" s="43" t="s">
         <v>45</v>
       </c>
-      <c r="E43" s="65"/>
-      <c r="F43" s="67"/>
-      <c r="G43" s="41"/>
+      <c r="E43" s="44"/>
+      <c r="F43" s="79"/>
+      <c r="G43" s="82"/>
     </row>
     <row r="44" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A44" s="79"/>
-      <c r="B44" s="60"/>
-      <c r="C44" s="61"/>
-      <c r="D44" s="64" t="s">
+      <c r="A44" s="70"/>
+      <c r="B44" s="88"/>
+      <c r="C44" s="89"/>
+      <c r="D44" s="43" t="s">
         <v>46</v>
       </c>
-      <c r="E44" s="65"/>
-      <c r="F44" s="67"/>
-      <c r="G44" s="41"/>
+      <c r="E44" s="44"/>
+      <c r="F44" s="79"/>
+      <c r="G44" s="82"/>
     </row>
     <row r="45" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A45" s="79"/>
-      <c r="B45" s="62"/>
-      <c r="C45" s="63"/>
-      <c r="D45" s="64" t="s">
+      <c r="A45" s="70"/>
+      <c r="B45" s="86"/>
+      <c r="C45" s="87"/>
+      <c r="D45" s="43" t="s">
         <v>47</v>
       </c>
-      <c r="E45" s="65"/>
-      <c r="F45" s="68"/>
-      <c r="G45" s="41"/>
+      <c r="E45" s="44"/>
+      <c r="F45" s="80"/>
+      <c r="G45" s="82"/>
     </row>
     <row r="46" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A46" s="79"/>
-      <c r="B46" s="58" t="s">
+      <c r="A46" s="70"/>
+      <c r="B46" s="84" t="s">
         <v>48</v>
       </c>
-      <c r="C46" s="59"/>
-      <c r="D46" s="64" t="s">
+      <c r="C46" s="85"/>
+      <c r="D46" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="E46" s="65"/>
-      <c r="F46" s="66">
+      <c r="E46" s="44"/>
+      <c r="F46" s="78">
         <v>2</v>
       </c>
-      <c r="G46" s="41"/>
+      <c r="G46" s="82"/>
     </row>
     <row r="47" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A47" s="79"/>
-      <c r="B47" s="60"/>
-      <c r="C47" s="61"/>
-      <c r="D47" s="64" t="s">
+      <c r="A47" s="70"/>
+      <c r="B47" s="88"/>
+      <c r="C47" s="89"/>
+      <c r="D47" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="E47" s="65"/>
-      <c r="F47" s="67"/>
-      <c r="G47" s="41"/>
+      <c r="E47" s="44"/>
+      <c r="F47" s="79"/>
+      <c r="G47" s="82"/>
     </row>
     <row r="48" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A48" s="79"/>
-      <c r="B48" s="60"/>
-      <c r="C48" s="61"/>
-      <c r="D48" s="64" t="s">
+      <c r="A48" s="70"/>
+      <c r="B48" s="88"/>
+      <c r="C48" s="89"/>
+      <c r="D48" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="E48" s="65"/>
-      <c r="F48" s="67"/>
-      <c r="G48" s="41"/>
+      <c r="E48" s="44"/>
+      <c r="F48" s="79"/>
+      <c r="G48" s="82"/>
     </row>
     <row r="49" spans="1:8" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A49" s="79"/>
-      <c r="B49" s="60"/>
-      <c r="C49" s="61"/>
-      <c r="D49" s="64" t="s">
+      <c r="A49" s="70"/>
+      <c r="B49" s="88"/>
+      <c r="C49" s="89"/>
+      <c r="D49" s="43" t="s">
         <v>53</v>
       </c>
-      <c r="E49" s="65"/>
-      <c r="F49" s="67"/>
-      <c r="G49" s="41"/>
+      <c r="E49" s="44"/>
+      <c r="F49" s="79"/>
+      <c r="G49" s="82"/>
     </row>
     <row r="50" spans="1:8" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A50" s="79"/>
-      <c r="B50" s="62"/>
-      <c r="C50" s="63"/>
-      <c r="D50" s="64" t="s">
+      <c r="A50" s="70"/>
+      <c r="B50" s="86"/>
+      <c r="C50" s="87"/>
+      <c r="D50" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="E50" s="65"/>
-      <c r="F50" s="68"/>
-      <c r="G50" s="41"/>
+      <c r="E50" s="44"/>
+      <c r="F50" s="80"/>
+      <c r="G50" s="82"/>
     </row>
     <row r="51" spans="1:8" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A51" s="79"/>
-      <c r="B51" s="58" t="s">
+      <c r="A51" s="70"/>
+      <c r="B51" s="84" t="s">
         <v>55</v>
       </c>
-      <c r="C51" s="59"/>
-      <c r="D51" s="64" t="s">
+      <c r="C51" s="85"/>
+      <c r="D51" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="E51" s="65"/>
-      <c r="F51" s="66">
+      <c r="E51" s="44"/>
+      <c r="F51" s="78">
         <v>2</v>
       </c>
-      <c r="G51" s="41"/>
+      <c r="G51" s="82"/>
     </row>
     <row r="52" spans="1:8" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A52" s="79"/>
-      <c r="B52" s="60"/>
-      <c r="C52" s="61"/>
-      <c r="D52" s="64" t="s">
+      <c r="A52" s="70"/>
+      <c r="B52" s="88"/>
+      <c r="C52" s="89"/>
+      <c r="D52" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="E52" s="65"/>
-      <c r="F52" s="67"/>
-      <c r="G52" s="41"/>
+      <c r="E52" s="44"/>
+      <c r="F52" s="79"/>
+      <c r="G52" s="82"/>
     </row>
     <row r="53" spans="1:8" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A53" s="79"/>
-      <c r="B53" s="60"/>
-      <c r="C53" s="61"/>
-      <c r="D53" s="64" t="s">
+      <c r="A53" s="70"/>
+      <c r="B53" s="88"/>
+      <c r="C53" s="89"/>
+      <c r="D53" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="E53" s="65"/>
-      <c r="F53" s="67"/>
-      <c r="G53" s="41"/>
+      <c r="E53" s="44"/>
+      <c r="F53" s="79"/>
+      <c r="G53" s="82"/>
     </row>
     <row r="54" spans="1:8" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A54" s="79"/>
-      <c r="B54" s="60"/>
-      <c r="C54" s="61"/>
-      <c r="D54" s="64" t="s">
+      <c r="A54" s="70"/>
+      <c r="B54" s="88"/>
+      <c r="C54" s="89"/>
+      <c r="D54" s="43" t="s">
         <v>57</v>
       </c>
-      <c r="E54" s="65"/>
-      <c r="F54" s="67"/>
-      <c r="G54" s="41"/>
+      <c r="E54" s="44"/>
+      <c r="F54" s="79"/>
+      <c r="G54" s="82"/>
     </row>
     <row r="55" spans="1:8" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A55" s="79"/>
-      <c r="B55" s="62"/>
-      <c r="C55" s="63"/>
-      <c r="D55" s="64" t="s">
+      <c r="A55" s="70"/>
+      <c r="B55" s="86"/>
+      <c r="C55" s="87"/>
+      <c r="D55" s="43" t="s">
         <v>58</v>
       </c>
-      <c r="E55" s="65"/>
-      <c r="F55" s="68"/>
-      <c r="G55" s="42"/>
+      <c r="E55" s="44"/>
+      <c r="F55" s="80"/>
+      <c r="G55" s="83"/>
     </row>
     <row r="56" spans="1:8" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A56" s="79"/>
-      <c r="B56" s="58" t="s">
+      <c r="A56" s="70"/>
+      <c r="B56" s="84" t="s">
         <v>59</v>
       </c>
-      <c r="C56" s="59"/>
-      <c r="D56" s="64" t="s">
+      <c r="C56" s="85"/>
+      <c r="D56" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="E56" s="65"/>
-      <c r="F56" s="66">
+      <c r="E56" s="44"/>
+      <c r="F56" s="78">
         <v>0</v>
       </c>
-      <c r="G56" s="40" t="s">
+      <c r="G56" s="81" t="s">
         <v>35</v>
       </c>
       <c r="H56" s="8"/>
     </row>
     <row r="57" spans="1:8" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A57" s="79"/>
-      <c r="B57" s="62"/>
-      <c r="C57" s="63"/>
-      <c r="D57" s="64" t="s">
+      <c r="A57" s="70"/>
+      <c r="B57" s="86"/>
+      <c r="C57" s="87"/>
+      <c r="D57" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="E57" s="65"/>
-      <c r="F57" s="68"/>
-      <c r="G57" s="42"/>
+      <c r="E57" s="44"/>
+      <c r="F57" s="80"/>
+      <c r="G57" s="83"/>
     </row>
     <row r="58" spans="1:8" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A58" s="79"/>
-      <c r="B58" s="58" t="s">
+      <c r="A58" s="70"/>
+      <c r="B58" s="84" t="s">
         <v>62</v>
       </c>
-      <c r="C58" s="59"/>
-      <c r="D58" s="64" t="s">
+      <c r="C58" s="85"/>
+      <c r="D58" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="E58" s="65"/>
-      <c r="F58" s="66">
+      <c r="E58" s="44"/>
+      <c r="F58" s="78">
         <v>0</v>
       </c>
-      <c r="G58" s="40" t="s">
+      <c r="G58" s="81" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="59" spans="1:8" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A59" s="79"/>
-      <c r="B59" s="62"/>
-      <c r="C59" s="63"/>
-      <c r="D59" s="64" t="s">
+      <c r="A59" s="70"/>
+      <c r="B59" s="86"/>
+      <c r="C59" s="87"/>
+      <c r="D59" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="E59" s="65"/>
-      <c r="F59" s="68"/>
-      <c r="G59" s="41"/>
+      <c r="E59" s="44"/>
+      <c r="F59" s="80"/>
+      <c r="G59" s="82"/>
     </row>
     <row r="60" spans="1:8" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A60" s="79"/>
-      <c r="B60" s="58" t="s">
+      <c r="A60" s="70"/>
+      <c r="B60" s="84" t="s">
         <v>65</v>
       </c>
-      <c r="C60" s="59"/>
-      <c r="D60" s="64" t="s">
+      <c r="C60" s="85"/>
+      <c r="D60" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="E60" s="65"/>
-      <c r="F60" s="66">
+      <c r="E60" s="44"/>
+      <c r="F60" s="78">
         <v>0</v>
       </c>
-      <c r="G60" s="41"/>
+      <c r="G60" s="82"/>
     </row>
     <row r="61" spans="1:8" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A61" s="79"/>
-      <c r="B61" s="60"/>
-      <c r="C61" s="61"/>
-      <c r="D61" s="64" t="s">
+      <c r="A61" s="70"/>
+      <c r="B61" s="88"/>
+      <c r="C61" s="89"/>
+      <c r="D61" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="E61" s="65"/>
-      <c r="F61" s="67"/>
-      <c r="G61" s="41"/>
+      <c r="E61" s="44"/>
+      <c r="F61" s="79"/>
+      <c r="G61" s="82"/>
     </row>
     <row r="62" spans="1:8" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A62" s="79"/>
-      <c r="B62" s="60"/>
-      <c r="C62" s="61"/>
-      <c r="D62" s="64" t="s">
+      <c r="A62" s="70"/>
+      <c r="B62" s="88"/>
+      <c r="C62" s="89"/>
+      <c r="D62" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="E62" s="65"/>
-      <c r="F62" s="67"/>
-      <c r="G62" s="41"/>
+      <c r="E62" s="44"/>
+      <c r="F62" s="79"/>
+      <c r="G62" s="82"/>
     </row>
     <row r="63" spans="1:8" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A63" s="79"/>
-      <c r="B63" s="60"/>
-      <c r="C63" s="61"/>
-      <c r="D63" s="64" t="s">
+      <c r="A63" s="70"/>
+      <c r="B63" s="88"/>
+      <c r="C63" s="89"/>
+      <c r="D63" s="43" t="s">
         <v>69</v>
       </c>
-      <c r="E63" s="65"/>
-      <c r="F63" s="67"/>
-      <c r="G63" s="41"/>
+      <c r="E63" s="44"/>
+      <c r="F63" s="79"/>
+      <c r="G63" s="82"/>
     </row>
     <row r="64" spans="1:8" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A64" s="79"/>
-      <c r="B64" s="60"/>
-      <c r="C64" s="61"/>
-      <c r="D64" s="64" t="s">
+      <c r="A64" s="70"/>
+      <c r="B64" s="88"/>
+      <c r="C64" s="89"/>
+      <c r="D64" s="43" t="s">
         <v>70</v>
       </c>
-      <c r="E64" s="65"/>
-      <c r="F64" s="67"/>
-      <c r="G64" s="41"/>
+      <c r="E64" s="44"/>
+      <c r="F64" s="79"/>
+      <c r="G64" s="82"/>
     </row>
     <row r="65" spans="1:7" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A65" s="80"/>
-      <c r="B65" s="62"/>
-      <c r="C65" s="63"/>
-      <c r="D65" s="64" t="s">
+      <c r="A65" s="71"/>
+      <c r="B65" s="86"/>
+      <c r="C65" s="87"/>
+      <c r="D65" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="E65" s="65"/>
-      <c r="F65" s="68"/>
-      <c r="G65" s="42"/>
+      <c r="E65" s="44"/>
+      <c r="F65" s="80"/>
+      <c r="G65" s="83"/>
     </row>
     <row r="66" spans="1:7" s="8" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A66" s="49" t="s">
+      <c r="A66" s="90" t="s">
         <v>72</v>
       </c>
-      <c r="B66" s="50" t="s">
+      <c r="B66" s="91" t="s">
         <v>73</v>
       </c>
-      <c r="C66" s="50"/>
-      <c r="D66" s="50" t="s">
+      <c r="C66" s="91"/>
+      <c r="D66" s="91" t="s">
         <v>74</v>
       </c>
-      <c r="E66" s="50"/>
+      <c r="E66" s="91"/>
       <c r="F66" s="17">
         <v>0</v>
       </c>
@@ -6061,15 +6069,15 @@
       </c>
     </row>
     <row r="67" spans="1:7" s="8" customFormat="1" ht="95.25" customHeight="1">
-      <c r="A67" s="49"/>
-      <c r="B67" s="51" t="s">
+      <c r="A67" s="90"/>
+      <c r="B67" s="92" t="s">
         <v>76</v>
       </c>
-      <c r="C67" s="51"/>
-      <c r="D67" s="47" t="s">
+      <c r="C67" s="92"/>
+      <c r="D67" s="93" t="s">
         <v>77</v>
       </c>
-      <c r="E67" s="47"/>
+      <c r="E67" s="93"/>
       <c r="F67" s="26">
         <v>0</v>
       </c>
@@ -6078,133 +6086,174 @@
       </c>
     </row>
     <row r="68" spans="1:7" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A68" s="49"/>
-      <c r="B68" s="52" t="s">
+      <c r="A68" s="90"/>
+      <c r="B68" s="94" t="s">
         <v>78</v>
       </c>
-      <c r="C68" s="53"/>
-      <c r="D68" s="43" t="s">
+      <c r="C68" s="95"/>
+      <c r="D68" s="100" t="s">
         <v>79</v>
       </c>
-      <c r="E68" s="44"/>
-      <c r="F68" s="37">
+      <c r="E68" s="101"/>
+      <c r="F68" s="103">
         <v>0</v>
       </c>
-      <c r="G68" s="40" t="s">
+      <c r="G68" s="81" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="69" spans="1:7" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A69" s="49"/>
-      <c r="B69" s="54"/>
-      <c r="C69" s="55"/>
-      <c r="D69" s="43" t="s">
+      <c r="A69" s="90"/>
+      <c r="B69" s="96"/>
+      <c r="C69" s="97"/>
+      <c r="D69" s="100" t="s">
         <v>81</v>
       </c>
-      <c r="E69" s="44"/>
-      <c r="F69" s="38"/>
-      <c r="G69" s="41"/>
+      <c r="E69" s="101"/>
+      <c r="F69" s="104"/>
+      <c r="G69" s="82"/>
     </row>
     <row r="70" spans="1:7" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A70" s="49"/>
-      <c r="B70" s="54"/>
-      <c r="C70" s="55"/>
-      <c r="D70" s="43" t="s">
+      <c r="A70" s="90"/>
+      <c r="B70" s="96"/>
+      <c r="C70" s="97"/>
+      <c r="D70" s="100" t="s">
         <v>82</v>
       </c>
-      <c r="E70" s="44"/>
-      <c r="F70" s="38"/>
-      <c r="G70" s="41"/>
+      <c r="E70" s="101"/>
+      <c r="F70" s="104"/>
+      <c r="G70" s="82"/>
     </row>
     <row r="71" spans="1:7" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A71" s="49"/>
-      <c r="B71" s="56"/>
-      <c r="C71" s="57"/>
-      <c r="D71" s="43" t="s">
+      <c r="A71" s="90"/>
+      <c r="B71" s="98"/>
+      <c r="C71" s="99"/>
+      <c r="D71" s="100" t="s">
         <v>83</v>
       </c>
-      <c r="E71" s="44"/>
-      <c r="F71" s="39"/>
-      <c r="G71" s="42"/>
+      <c r="E71" s="101"/>
+      <c r="F71" s="105"/>
+      <c r="G71" s="83"/>
     </row>
     <row r="72" spans="1:7" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A72" s="49"/>
-      <c r="B72" s="45" t="s">
+      <c r="A72" s="90"/>
+      <c r="B72" s="102" t="s">
         <v>84</v>
       </c>
-      <c r="C72" s="45"/>
-      <c r="D72" s="45" t="s">
+      <c r="C72" s="102"/>
+      <c r="D72" s="102" t="s">
         <v>85</v>
       </c>
-      <c r="E72" s="45"/>
-      <c r="F72" s="46">
+      <c r="E72" s="102"/>
+      <c r="F72" s="106">
         <v>0</v>
       </c>
-      <c r="G72" s="47" t="s">
+      <c r="G72" s="93" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="73" spans="1:7" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A73" s="49"/>
-      <c r="B73" s="45"/>
-      <c r="C73" s="45"/>
-      <c r="D73" s="48" t="s">
+      <c r="A73" s="90"/>
+      <c r="B73" s="102"/>
+      <c r="C73" s="102"/>
+      <c r="D73" s="107" t="s">
         <v>87</v>
       </c>
-      <c r="E73" s="48"/>
-      <c r="F73" s="46"/>
-      <c r="G73" s="47"/>
+      <c r="E73" s="107"/>
+      <c r="F73" s="106"/>
+      <c r="G73" s="93"/>
     </row>
     <row r="74" spans="1:7" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A74" s="49"/>
-      <c r="B74" s="45"/>
-      <c r="C74" s="45"/>
-      <c r="D74" s="45" t="s">
+      <c r="A74" s="90"/>
+      <c r="B74" s="102"/>
+      <c r="C74" s="102"/>
+      <c r="D74" s="102" t="s">
         <v>88</v>
       </c>
-      <c r="E74" s="45"/>
-      <c r="F74" s="46"/>
-      <c r="G74" s="47"/>
+      <c r="E74" s="102"/>
+      <c r="F74" s="106"/>
+      <c r="G74" s="93"/>
     </row>
     <row r="75" spans="1:7" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A75" s="49"/>
-      <c r="B75" s="45"/>
-      <c r="C75" s="45"/>
-      <c r="D75" s="45" t="s">
+      <c r="A75" s="90"/>
+      <c r="B75" s="102"/>
+      <c r="C75" s="102"/>
+      <c r="D75" s="102" t="s">
         <v>89</v>
       </c>
-      <c r="E75" s="45"/>
-      <c r="F75" s="46"/>
-      <c r="G75" s="47"/>
+      <c r="E75" s="102"/>
+      <c r="F75" s="106"/>
+      <c r="G75" s="93"/>
     </row>
   </sheetData>
   <mergeCells count="117">
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:A20"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="B7:B20"/>
-    <mergeCell ref="D7:G7"/>
-    <mergeCell ref="D17:G17"/>
-    <mergeCell ref="D18:G18"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:G19"/>
-    <mergeCell ref="D20:G20"/>
-    <mergeCell ref="A21:G21"/>
-    <mergeCell ref="C8:C18"/>
-    <mergeCell ref="D8:G8"/>
-    <mergeCell ref="D9:G9"/>
-    <mergeCell ref="D10:G10"/>
-    <mergeCell ref="D11:G11"/>
-    <mergeCell ref="D12:G12"/>
-    <mergeCell ref="D13:G13"/>
-    <mergeCell ref="D14:G14"/>
-    <mergeCell ref="D15:G15"/>
-    <mergeCell ref="D16:G16"/>
+    <mergeCell ref="G68:G71"/>
+    <mergeCell ref="D69:E69"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="B72:C75"/>
+    <mergeCell ref="D72:E72"/>
+    <mergeCell ref="F72:F75"/>
+    <mergeCell ref="G72:G75"/>
+    <mergeCell ref="D73:E73"/>
+    <mergeCell ref="F56:F57"/>
+    <mergeCell ref="A66:A75"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="D67:E67"/>
+    <mergeCell ref="B68:C71"/>
+    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="D74:E74"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="F68:F71"/>
+    <mergeCell ref="G56:G57"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="B58:C59"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="F58:F59"/>
+    <mergeCell ref="G58:G65"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="B51:C55"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="F51:F55"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="B60:C65"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="F60:F65"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="B56:C57"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="B36:C40"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="F36:F40"/>
+    <mergeCell ref="G36:G55"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="B46:C50"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="F46:F50"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="B41:C45"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:F45"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D45:E45"/>
     <mergeCell ref="B22:C22"/>
     <mergeCell ref="D22:E22"/>
     <mergeCell ref="A23:A65"/>
@@ -6229,73 +6278,32 @@
     <mergeCell ref="B29:C33"/>
     <mergeCell ref="D29:E29"/>
     <mergeCell ref="G34:G35"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="B36:C40"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="F36:F40"/>
-    <mergeCell ref="G36:G55"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="B46:C50"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="F46:F50"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="B41:C45"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:F45"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="G56:G57"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="B58:C59"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="F58:F59"/>
-    <mergeCell ref="G58:G65"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="B51:C55"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="F51:F55"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="B60:C65"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="F60:F65"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="D63:E63"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="B56:C57"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="F56:F57"/>
-    <mergeCell ref="A66:A75"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="D67:E67"/>
-    <mergeCell ref="B68:C71"/>
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="D74:E74"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="F68:F71"/>
-    <mergeCell ref="G68:G71"/>
-    <mergeCell ref="D69:E69"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="B72:C75"/>
-    <mergeCell ref="D72:E72"/>
-    <mergeCell ref="F72:F75"/>
-    <mergeCell ref="G72:G75"/>
-    <mergeCell ref="D73:E73"/>
+    <mergeCell ref="A21:G21"/>
+    <mergeCell ref="C8:C18"/>
+    <mergeCell ref="D8:G8"/>
+    <mergeCell ref="D9:G9"/>
+    <mergeCell ref="D10:G10"/>
+    <mergeCell ref="D11:G11"/>
+    <mergeCell ref="D12:G12"/>
+    <mergeCell ref="D13:G13"/>
+    <mergeCell ref="D14:G14"/>
+    <mergeCell ref="D15:G15"/>
+    <mergeCell ref="D16:G16"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:A20"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="B7:B20"/>
+    <mergeCell ref="D7:G7"/>
+    <mergeCell ref="D17:G17"/>
+    <mergeCell ref="D18:G18"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:G19"/>
+    <mergeCell ref="D20:G20"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="F66">
@@ -6357,15 +6365,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="1" customFormat="1" ht="32.25" customHeight="1">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="91"/>
-      <c r="C1" s="91"/>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91"/>
-      <c r="F1" s="91"/>
-      <c r="G1" s="91"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
       <c r="J1" s="2"/>
       <c r="L1" s="3"/>
       <c r="M1" s="4"/>
@@ -6374,15 +6382,15 @@
       <c r="P1" s="4"/>
     </row>
     <row r="2" spans="1:17" s="1" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A2" s="92" t="s">
+      <c r="A2" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="92"/>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="92"/>
-      <c r="F2" s="92"/>
-      <c r="G2" s="92"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
       <c r="J2" s="2"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
@@ -6395,10 +6403,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="5"/>
-      <c r="C3" s="92" t="s">
+      <c r="C3" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="92"/>
+      <c r="D3" s="47"/>
       <c r="E3" s="6"/>
       <c r="F3" s="5" t="s">
         <v>4</v>
@@ -6416,10 +6424,10 @@
         <v>5</v>
       </c>
       <c r="B4" s="5"/>
-      <c r="C4" s="92" t="s">
+      <c r="C4" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="92"/>
+      <c r="D4" s="47"/>
       <c r="E4" s="10"/>
       <c r="F4" s="11" t="s">
         <v>7</v>
@@ -6433,19 +6441,19 @@
       <c r="Q4" s="4"/>
     </row>
     <row r="5" spans="1:17" s="8" customFormat="1" ht="49.5" customHeight="1">
-      <c r="A5" s="93" t="s">
+      <c r="A5" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="87" t="s">
+      <c r="B5" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="96">
+      <c r="C5" s="52">
         <v>6</v>
       </c>
-      <c r="D5" s="97"/>
-      <c r="E5" s="97"/>
-      <c r="F5" s="97"/>
-      <c r="G5" s="98"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="54"/>
       <c r="H5" s="31"/>
       <c r="J5" s="12"/>
       <c r="K5" s="4"/>
@@ -6457,28 +6465,28 @@
       <c r="Q5" s="4"/>
     </row>
     <row r="6" spans="1:17" s="13" customFormat="1" ht="48" customHeight="1">
-      <c r="A6" s="94"/>
-      <c r="B6" s="95"/>
-      <c r="C6" s="104"/>
-      <c r="D6" s="105"/>
-      <c r="E6" s="105"/>
-      <c r="F6" s="105"/>
-      <c r="G6" s="106"/>
+      <c r="A6" s="49"/>
+      <c r="B6" s="51"/>
+      <c r="C6" s="59"/>
+      <c r="D6" s="60"/>
+      <c r="E6" s="60"/>
+      <c r="F6" s="60"/>
+      <c r="G6" s="61"/>
       <c r="I6" s="14"/>
       <c r="J6" s="14"/>
       <c r="K6" s="14"/>
       <c r="L6" s="14"/>
     </row>
     <row r="7" spans="1:17" s="8" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A7" s="75" t="s">
+      <c r="A7" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="89"/>
-      <c r="C7" s="89"/>
-      <c r="D7" s="89"/>
-      <c r="E7" s="89"/>
-      <c r="F7" s="89"/>
-      <c r="G7" s="76"/>
+      <c r="B7" s="45"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="39"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
@@ -6488,14 +6496,14 @@
       <c r="A8" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="75" t="s">
+      <c r="B8" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="76"/>
-      <c r="D8" s="77" t="s">
+      <c r="C8" s="39"/>
+      <c r="D8" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="77"/>
+      <c r="E8" s="40"/>
       <c r="F8" s="16" t="s">
         <v>14</v>
       </c>
@@ -6508,17 +6516,17 @@
       <c r="L8" s="4"/>
     </row>
     <row r="9" spans="1:17" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A9" s="78" t="s">
+      <c r="A9" s="69" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="81" t="s">
+      <c r="B9" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="82"/>
-      <c r="D9" s="64" t="s">
+      <c r="C9" s="42"/>
+      <c r="D9" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="65"/>
+      <c r="E9" s="44"/>
       <c r="F9" s="17"/>
       <c r="G9" s="18" t="s">
         <v>19</v>
@@ -6528,19 +6536,19 @@
       <c r="K9" s="4"/>
     </row>
     <row r="10" spans="1:17" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A10" s="79"/>
-      <c r="B10" s="69" t="s">
+      <c r="A10" s="70"/>
+      <c r="B10" s="72" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="70"/>
-      <c r="D10" s="64" t="s">
+      <c r="C10" s="73"/>
+      <c r="D10" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="65"/>
-      <c r="F10" s="66">
+      <c r="E10" s="44"/>
+      <c r="F10" s="78">
         <v>2</v>
       </c>
-      <c r="G10" s="107" t="s">
+      <c r="G10" s="108" t="s">
         <v>22</v>
       </c>
       <c r="K10" s="4"/>
@@ -6549,79 +6557,79 @@
       <c r="N10" s="4"/>
     </row>
     <row r="11" spans="1:17" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A11" s="79"/>
-      <c r="B11" s="71"/>
-      <c r="C11" s="72"/>
-      <c r="D11" s="64" t="s">
+      <c r="A11" s="70"/>
+      <c r="B11" s="74"/>
+      <c r="C11" s="75"/>
+      <c r="D11" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="65"/>
-      <c r="F11" s="67"/>
-      <c r="G11" s="108"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="79"/>
+      <c r="G11" s="109"/>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
       <c r="M11" s="4"/>
       <c r="N11" s="4"/>
     </row>
     <row r="12" spans="1:17" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A12" s="79"/>
-      <c r="B12" s="71"/>
-      <c r="C12" s="72"/>
-      <c r="D12" s="64" t="s">
+      <c r="A12" s="70"/>
+      <c r="B12" s="74"/>
+      <c r="C12" s="75"/>
+      <c r="D12" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="E12" s="65"/>
-      <c r="F12" s="67"/>
-      <c r="G12" s="108"/>
+      <c r="E12" s="44"/>
+      <c r="F12" s="79"/>
+      <c r="G12" s="109"/>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
     </row>
     <row r="13" spans="1:17" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A13" s="79"/>
-      <c r="B13" s="71"/>
-      <c r="C13" s="72"/>
-      <c r="D13" s="64" t="s">
+      <c r="A13" s="70"/>
+      <c r="B13" s="74"/>
+      <c r="C13" s="75"/>
+      <c r="D13" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="65"/>
-      <c r="F13" s="67"/>
-      <c r="G13" s="108"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="79"/>
+      <c r="G13" s="109"/>
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
     </row>
     <row r="14" spans="1:17" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A14" s="79"/>
-      <c r="B14" s="73"/>
-      <c r="C14" s="74"/>
-      <c r="D14" s="64" t="s">
+      <c r="A14" s="70"/>
+      <c r="B14" s="76"/>
+      <c r="C14" s="77"/>
+      <c r="D14" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="65"/>
-      <c r="F14" s="68"/>
-      <c r="G14" s="108"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="80"/>
+      <c r="G14" s="109"/>
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
     </row>
     <row r="15" spans="1:17" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A15" s="79"/>
-      <c r="B15" s="58" t="s">
+      <c r="A15" s="70"/>
+      <c r="B15" s="84" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="59"/>
-      <c r="D15" s="64" t="s">
+      <c r="C15" s="85"/>
+      <c r="D15" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="65"/>
-      <c r="F15" s="66">
+      <c r="E15" s="44"/>
+      <c r="F15" s="78">
         <v>2</v>
       </c>
-      <c r="G15" s="108"/>
+      <c r="G15" s="109"/>
       <c r="H15" s="19"/>
       <c r="I15" s="19"/>
       <c r="J15" s="19"/>
@@ -6631,15 +6639,15 @@
       <c r="N15" s="4"/>
     </row>
     <row r="16" spans="1:17" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A16" s="79"/>
-      <c r="B16" s="60"/>
-      <c r="C16" s="61"/>
-      <c r="D16" s="64" t="s">
+      <c r="A16" s="70"/>
+      <c r="B16" s="88"/>
+      <c r="C16" s="89"/>
+      <c r="D16" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="E16" s="65"/>
-      <c r="F16" s="67"/>
-      <c r="G16" s="108"/>
+      <c r="E16" s="44"/>
+      <c r="F16" s="79"/>
+      <c r="G16" s="109"/>
       <c r="H16" s="19"/>
       <c r="I16" s="19"/>
       <c r="J16" s="19"/>
@@ -6649,15 +6657,15 @@
       <c r="N16" s="4"/>
     </row>
     <row r="17" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A17" s="79"/>
-      <c r="B17" s="60"/>
-      <c r="C17" s="61"/>
-      <c r="D17" s="64" t="s">
+      <c r="A17" s="70"/>
+      <c r="B17" s="88"/>
+      <c r="C17" s="89"/>
+      <c r="D17" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="E17" s="65"/>
-      <c r="F17" s="67"/>
-      <c r="G17" s="108"/>
+      <c r="E17" s="44"/>
+      <c r="F17" s="79"/>
+      <c r="G17" s="109"/>
       <c r="H17" s="19"/>
       <c r="I17" s="19"/>
       <c r="J17" s="19"/>
@@ -6667,15 +6675,15 @@
       <c r="N17" s="4"/>
     </row>
     <row r="18" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A18" s="79"/>
-      <c r="B18" s="60"/>
-      <c r="C18" s="61"/>
-      <c r="D18" s="64" t="s">
+      <c r="A18" s="70"/>
+      <c r="B18" s="88"/>
+      <c r="C18" s="89"/>
+      <c r="D18" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="E18" s="65"/>
-      <c r="F18" s="67"/>
-      <c r="G18" s="108"/>
+      <c r="E18" s="44"/>
+      <c r="F18" s="79"/>
+      <c r="G18" s="109"/>
       <c r="H18" s="19"/>
       <c r="I18" s="19"/>
       <c r="J18" s="19"/>
@@ -6685,15 +6693,15 @@
       <c r="N18" s="4"/>
     </row>
     <row r="19" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A19" s="79"/>
-      <c r="B19" s="62"/>
-      <c r="C19" s="63"/>
-      <c r="D19" s="64" t="s">
+      <c r="A19" s="70"/>
+      <c r="B19" s="86"/>
+      <c r="C19" s="87"/>
+      <c r="D19" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="E19" s="65"/>
-      <c r="F19" s="68"/>
-      <c r="G19" s="109"/>
+      <c r="E19" s="44"/>
+      <c r="F19" s="80"/>
+      <c r="G19" s="110"/>
       <c r="H19" s="19"/>
       <c r="I19" s="19"/>
       <c r="J19" s="19"/>
@@ -6703,19 +6711,19 @@
       <c r="N19" s="4"/>
     </row>
     <row r="20" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A20" s="79"/>
-      <c r="B20" s="58" t="s">
+      <c r="A20" s="70"/>
+      <c r="B20" s="84" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="59"/>
-      <c r="D20" s="64" t="s">
+      <c r="C20" s="85"/>
+      <c r="D20" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="E20" s="65"/>
-      <c r="F20" s="66">
+      <c r="E20" s="44"/>
+      <c r="F20" s="78">
         <v>0</v>
       </c>
-      <c r="G20" s="107" t="s">
+      <c r="G20" s="108" t="s">
         <v>35</v>
       </c>
       <c r="K20" s="4"/>
@@ -6724,34 +6732,34 @@
       <c r="N20" s="4"/>
     </row>
     <row r="21" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A21" s="79"/>
-      <c r="B21" s="62"/>
-      <c r="C21" s="63"/>
-      <c r="D21" s="64" t="s">
+      <c r="A21" s="70"/>
+      <c r="B21" s="86"/>
+      <c r="C21" s="87"/>
+      <c r="D21" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="E21" s="65"/>
-      <c r="F21" s="68"/>
-      <c r="G21" s="109"/>
+      <c r="E21" s="44"/>
+      <c r="F21" s="80"/>
+      <c r="G21" s="110"/>
       <c r="K21" s="4"/>
       <c r="L21" s="4"/>
       <c r="M21" s="4"/>
       <c r="N21" s="4"/>
     </row>
     <row r="22" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A22" s="79"/>
-      <c r="B22" s="69" t="s">
+      <c r="A22" s="70"/>
+      <c r="B22" s="72" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="70"/>
-      <c r="D22" s="64" t="s">
+      <c r="C22" s="73"/>
+      <c r="D22" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="E22" s="65"/>
-      <c r="F22" s="66">
+      <c r="E22" s="44"/>
+      <c r="F22" s="78">
         <v>2</v>
       </c>
-      <c r="G22" s="40" t="s">
+      <c r="G22" s="81" t="s">
         <v>22</v>
       </c>
       <c r="K22" s="4"/>
@@ -6760,79 +6768,79 @@
       <c r="N22" s="4"/>
     </row>
     <row r="23" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A23" s="79"/>
-      <c r="B23" s="71"/>
-      <c r="C23" s="72"/>
-      <c r="D23" s="64" t="s">
+      <c r="A23" s="70"/>
+      <c r="B23" s="74"/>
+      <c r="C23" s="75"/>
+      <c r="D23" s="43" t="s">
         <v>38</v>
       </c>
-      <c r="E23" s="65"/>
-      <c r="F23" s="67"/>
-      <c r="G23" s="41"/>
+      <c r="E23" s="44"/>
+      <c r="F23" s="79"/>
+      <c r="G23" s="82"/>
       <c r="K23" s="4"/>
       <c r="L23" s="4"/>
       <c r="M23" s="4"/>
       <c r="N23" s="4"/>
     </row>
     <row r="24" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A24" s="79"/>
-      <c r="B24" s="71"/>
-      <c r="C24" s="72"/>
-      <c r="D24" s="64" t="s">
+      <c r="A24" s="70"/>
+      <c r="B24" s="74"/>
+      <c r="C24" s="75"/>
+      <c r="D24" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="E24" s="65"/>
-      <c r="F24" s="67"/>
-      <c r="G24" s="41"/>
+      <c r="E24" s="44"/>
+      <c r="F24" s="79"/>
+      <c r="G24" s="82"/>
       <c r="K24" s="4"/>
       <c r="L24" s="4"/>
       <c r="M24" s="4"/>
       <c r="N24" s="4"/>
     </row>
     <row r="25" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A25" s="79"/>
-      <c r="B25" s="71"/>
-      <c r="C25" s="72"/>
-      <c r="D25" s="64" t="s">
+      <c r="A25" s="70"/>
+      <c r="B25" s="74"/>
+      <c r="C25" s="75"/>
+      <c r="D25" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="E25" s="65"/>
-      <c r="F25" s="67"/>
-      <c r="G25" s="41"/>
+      <c r="E25" s="44"/>
+      <c r="F25" s="79"/>
+      <c r="G25" s="82"/>
       <c r="K25" s="4"/>
       <c r="L25" s="4"/>
       <c r="M25" s="4"/>
       <c r="N25" s="4"/>
     </row>
     <row r="26" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A26" s="79"/>
-      <c r="B26" s="73"/>
-      <c r="C26" s="74"/>
-      <c r="D26" s="64" t="s">
+      <c r="A26" s="70"/>
+      <c r="B26" s="76"/>
+      <c r="C26" s="77"/>
+      <c r="D26" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="E26" s="65"/>
-      <c r="F26" s="68"/>
-      <c r="G26" s="41"/>
+      <c r="E26" s="44"/>
+      <c r="F26" s="80"/>
+      <c r="G26" s="82"/>
       <c r="K26" s="4"/>
       <c r="L26" s="4"/>
       <c r="M26" s="4"/>
       <c r="P26" s="4"/>
     </row>
     <row r="27" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A27" s="79"/>
-      <c r="B27" s="58" t="s">
+      <c r="A27" s="70"/>
+      <c r="B27" s="84" t="s">
         <v>42</v>
       </c>
-      <c r="C27" s="59"/>
-      <c r="D27" s="64" t="s">
+      <c r="C27" s="85"/>
+      <c r="D27" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="E27" s="65"/>
-      <c r="F27" s="66">
+      <c r="E27" s="44"/>
+      <c r="F27" s="78">
         <v>2</v>
       </c>
-      <c r="G27" s="41"/>
+      <c r="G27" s="82"/>
       <c r="H27" s="19"/>
       <c r="I27" s="19"/>
       <c r="J27" s="19"/>
@@ -6842,15 +6850,15 @@
       <c r="N27" s="4"/>
     </row>
     <row r="28" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A28" s="79"/>
-      <c r="B28" s="60"/>
-      <c r="C28" s="61"/>
-      <c r="D28" s="64" t="s">
+      <c r="A28" s="70"/>
+      <c r="B28" s="88"/>
+      <c r="C28" s="89"/>
+      <c r="D28" s="43" t="s">
         <v>44</v>
       </c>
-      <c r="E28" s="65"/>
-      <c r="F28" s="67"/>
-      <c r="G28" s="41"/>
+      <c r="E28" s="44"/>
+      <c r="F28" s="79"/>
+      <c r="G28" s="82"/>
       <c r="H28" s="19"/>
       <c r="I28" s="19"/>
       <c r="J28" s="19"/>
@@ -6859,15 +6867,15 @@
       <c r="M28" s="20"/>
     </row>
     <row r="29" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A29" s="79"/>
-      <c r="B29" s="60"/>
-      <c r="C29" s="61"/>
-      <c r="D29" s="64" t="s">
+      <c r="A29" s="70"/>
+      <c r="B29" s="88"/>
+      <c r="C29" s="89"/>
+      <c r="D29" s="43" t="s">
         <v>45</v>
       </c>
-      <c r="E29" s="65"/>
-      <c r="F29" s="67"/>
-      <c r="G29" s="41"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="79"/>
+      <c r="G29" s="82"/>
       <c r="H29" s="19"/>
       <c r="I29" s="19"/>
       <c r="J29" s="19"/>
@@ -6876,15 +6884,15 @@
       <c r="M29" s="20"/>
     </row>
     <row r="30" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A30" s="79"/>
-      <c r="B30" s="60"/>
-      <c r="C30" s="61"/>
-      <c r="D30" s="64" t="s">
+      <c r="A30" s="70"/>
+      <c r="B30" s="88"/>
+      <c r="C30" s="89"/>
+      <c r="D30" s="43" t="s">
         <v>46</v>
       </c>
-      <c r="E30" s="65"/>
-      <c r="F30" s="67"/>
-      <c r="G30" s="41"/>
+      <c r="E30" s="44"/>
+      <c r="F30" s="79"/>
+      <c r="G30" s="82"/>
       <c r="H30" s="19"/>
       <c r="I30" s="19"/>
       <c r="J30" s="19"/>
@@ -6893,15 +6901,15 @@
       <c r="M30" s="20"/>
     </row>
     <row r="31" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A31" s="79"/>
-      <c r="B31" s="62"/>
-      <c r="C31" s="63"/>
-      <c r="D31" s="64" t="s">
+      <c r="A31" s="70"/>
+      <c r="B31" s="86"/>
+      <c r="C31" s="87"/>
+      <c r="D31" s="43" t="s">
         <v>47</v>
       </c>
-      <c r="E31" s="65"/>
-      <c r="F31" s="68"/>
-      <c r="G31" s="41"/>
+      <c r="E31" s="44"/>
+      <c r="F31" s="80"/>
+      <c r="G31" s="82"/>
       <c r="H31" s="19"/>
       <c r="I31" s="19"/>
       <c r="J31" s="19"/>
@@ -6910,19 +6918,19 @@
       <c r="M31" s="20"/>
     </row>
     <row r="32" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A32" s="79"/>
-      <c r="B32" s="58" t="s">
+      <c r="A32" s="70"/>
+      <c r="B32" s="84" t="s">
         <v>48</v>
       </c>
-      <c r="C32" s="59"/>
-      <c r="D32" s="64" t="s">
+      <c r="C32" s="85"/>
+      <c r="D32" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="E32" s="65"/>
-      <c r="F32" s="66">
+      <c r="E32" s="44"/>
+      <c r="F32" s="78">
         <v>2</v>
       </c>
-      <c r="G32" s="41" t="s">
+      <c r="G32" s="82" t="s">
         <v>50</v>
       </c>
       <c r="H32" s="19"/>
@@ -6934,15 +6942,15 @@
       <c r="N32" s="4"/>
     </row>
     <row r="33" spans="1:15" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A33" s="79"/>
-      <c r="B33" s="60"/>
-      <c r="C33" s="61"/>
-      <c r="D33" s="64" t="s">
+      <c r="A33" s="70"/>
+      <c r="B33" s="88"/>
+      <c r="C33" s="89"/>
+      <c r="D33" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="E33" s="65"/>
-      <c r="F33" s="67"/>
-      <c r="G33" s="41"/>
+      <c r="E33" s="44"/>
+      <c r="F33" s="79"/>
+      <c r="G33" s="82"/>
       <c r="H33" s="19"/>
       <c r="I33" s="19"/>
       <c r="J33" s="19"/>
@@ -6952,15 +6960,15 @@
       <c r="N33" s="4"/>
     </row>
     <row r="34" spans="1:15" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A34" s="79"/>
-      <c r="B34" s="60"/>
-      <c r="C34" s="61"/>
-      <c r="D34" s="64" t="s">
+      <c r="A34" s="70"/>
+      <c r="B34" s="88"/>
+      <c r="C34" s="89"/>
+      <c r="D34" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="E34" s="65"/>
-      <c r="F34" s="67"/>
-      <c r="G34" s="41"/>
+      <c r="E34" s="44"/>
+      <c r="F34" s="79"/>
+      <c r="G34" s="82"/>
       <c r="H34" s="19"/>
       <c r="I34" s="19"/>
       <c r="J34" s="19"/>
@@ -6970,15 +6978,15 @@
       <c r="N34" s="4"/>
     </row>
     <row r="35" spans="1:15" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A35" s="79"/>
-      <c r="B35" s="60"/>
-      <c r="C35" s="61"/>
-      <c r="D35" s="64" t="s">
+      <c r="A35" s="70"/>
+      <c r="B35" s="88"/>
+      <c r="C35" s="89"/>
+      <c r="D35" s="43" t="s">
         <v>53</v>
       </c>
-      <c r="E35" s="65"/>
-      <c r="F35" s="67"/>
-      <c r="G35" s="41"/>
+      <c r="E35" s="44"/>
+      <c r="F35" s="79"/>
+      <c r="G35" s="82"/>
       <c r="H35" s="19"/>
       <c r="I35" s="19"/>
       <c r="J35" s="19"/>
@@ -6988,15 +6996,15 @@
       <c r="N35" s="4"/>
     </row>
     <row r="36" spans="1:15" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A36" s="79"/>
-      <c r="B36" s="62"/>
-      <c r="C36" s="63"/>
-      <c r="D36" s="64" t="s">
+      <c r="A36" s="70"/>
+      <c r="B36" s="86"/>
+      <c r="C36" s="87"/>
+      <c r="D36" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="E36" s="65"/>
-      <c r="F36" s="68"/>
-      <c r="G36" s="41"/>
+      <c r="E36" s="44"/>
+      <c r="F36" s="80"/>
+      <c r="G36" s="82"/>
       <c r="H36" s="19"/>
       <c r="I36" s="19"/>
       <c r="J36" s="19"/>
@@ -7006,98 +7014,98 @@
       <c r="N36" s="4"/>
     </row>
     <row r="37" spans="1:15" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A37" s="79"/>
-      <c r="B37" s="58" t="s">
+      <c r="A37" s="70"/>
+      <c r="B37" s="84" t="s">
         <v>55</v>
       </c>
-      <c r="C37" s="59"/>
-      <c r="D37" s="64" t="s">
+      <c r="C37" s="85"/>
+      <c r="D37" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="E37" s="65"/>
-      <c r="F37" s="66">
+      <c r="E37" s="44"/>
+      <c r="F37" s="78">
         <v>2</v>
       </c>
-      <c r="G37" s="41"/>
+      <c r="G37" s="82"/>
       <c r="K37" s="4"/>
       <c r="L37" s="4"/>
       <c r="M37" s="4"/>
       <c r="N37" s="4"/>
     </row>
     <row r="38" spans="1:15" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A38" s="79"/>
-      <c r="B38" s="60"/>
-      <c r="C38" s="61"/>
-      <c r="D38" s="64" t="s">
+      <c r="A38" s="70"/>
+      <c r="B38" s="88"/>
+      <c r="C38" s="89"/>
+      <c r="D38" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="E38" s="65"/>
-      <c r="F38" s="67"/>
-      <c r="G38" s="41"/>
+      <c r="E38" s="44"/>
+      <c r="F38" s="79"/>
+      <c r="G38" s="82"/>
       <c r="K38" s="4"/>
       <c r="L38" s="4"/>
       <c r="M38" s="4"/>
       <c r="N38" s="4"/>
     </row>
     <row r="39" spans="1:15" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A39" s="79"/>
-      <c r="B39" s="60"/>
-      <c r="C39" s="61"/>
-      <c r="D39" s="64" t="s">
+      <c r="A39" s="70"/>
+      <c r="B39" s="88"/>
+      <c r="C39" s="89"/>
+      <c r="D39" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="E39" s="65"/>
-      <c r="F39" s="67"/>
-      <c r="G39" s="41"/>
+      <c r="E39" s="44"/>
+      <c r="F39" s="79"/>
+      <c r="G39" s="82"/>
       <c r="K39" s="4"/>
       <c r="L39" s="4"/>
       <c r="M39" s="4"/>
       <c r="N39" s="4"/>
     </row>
     <row r="40" spans="1:15" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A40" s="79"/>
-      <c r="B40" s="60"/>
-      <c r="C40" s="61"/>
-      <c r="D40" s="64" t="s">
+      <c r="A40" s="70"/>
+      <c r="B40" s="88"/>
+      <c r="C40" s="89"/>
+      <c r="D40" s="43" t="s">
         <v>57</v>
       </c>
-      <c r="E40" s="65"/>
-      <c r="F40" s="67"/>
-      <c r="G40" s="41"/>
+      <c r="E40" s="44"/>
+      <c r="F40" s="79"/>
+      <c r="G40" s="82"/>
       <c r="K40" s="21"/>
       <c r="L40" s="21"/>
       <c r="M40" s="4"/>
       <c r="N40" s="4"/>
     </row>
     <row r="41" spans="1:15" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A41" s="79"/>
-      <c r="B41" s="62"/>
-      <c r="C41" s="63"/>
-      <c r="D41" s="64" t="s">
+      <c r="A41" s="70"/>
+      <c r="B41" s="86"/>
+      <c r="C41" s="87"/>
+      <c r="D41" s="43" t="s">
         <v>58</v>
       </c>
-      <c r="E41" s="65"/>
-      <c r="F41" s="68"/>
-      <c r="G41" s="42"/>
+      <c r="E41" s="44"/>
+      <c r="F41" s="80"/>
+      <c r="G41" s="83"/>
       <c r="K41" s="4"/>
       <c r="L41" s="4"/>
       <c r="M41" s="4"/>
       <c r="N41" s="4"/>
     </row>
     <row r="42" spans="1:15" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A42" s="79"/>
-      <c r="B42" s="58" t="s">
+      <c r="A42" s="70"/>
+      <c r="B42" s="84" t="s">
         <v>59</v>
       </c>
-      <c r="C42" s="59"/>
-      <c r="D42" s="64" t="s">
+      <c r="C42" s="85"/>
+      <c r="D42" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="E42" s="65"/>
-      <c r="F42" s="66">
+      <c r="E42" s="44"/>
+      <c r="F42" s="78">
         <v>0</v>
       </c>
-      <c r="G42" s="40" t="s">
+      <c r="G42" s="81" t="s">
         <v>35</v>
       </c>
       <c r="K42" s="21"/>
@@ -7107,34 +7115,34 @@
       <c r="O42" s="8"/>
     </row>
     <row r="43" spans="1:15" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A43" s="79"/>
-      <c r="B43" s="62"/>
-      <c r="C43" s="63"/>
-      <c r="D43" s="64" t="s">
+      <c r="A43" s="70"/>
+      <c r="B43" s="86"/>
+      <c r="C43" s="87"/>
+      <c r="D43" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="E43" s="65"/>
-      <c r="F43" s="68"/>
-      <c r="G43" s="42"/>
+      <c r="E43" s="44"/>
+      <c r="F43" s="80"/>
+      <c r="G43" s="83"/>
       <c r="K43" s="21"/>
       <c r="L43" s="21"/>
       <c r="M43" s="21"/>
       <c r="N43" s="21"/>
     </row>
     <row r="44" spans="1:15" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A44" s="79"/>
-      <c r="B44" s="58" t="s">
+      <c r="A44" s="70"/>
+      <c r="B44" s="84" t="s">
         <v>62</v>
       </c>
-      <c r="C44" s="59"/>
-      <c r="D44" s="64" t="s">
+      <c r="C44" s="85"/>
+      <c r="D44" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="E44" s="65"/>
-      <c r="F44" s="66">
+      <c r="E44" s="44"/>
+      <c r="F44" s="78">
         <v>0</v>
       </c>
-      <c r="G44" s="40" t="s">
+      <c r="G44" s="81" t="s">
         <v>22</v>
       </c>
       <c r="H44" s="8"/>
@@ -7146,15 +7154,15 @@
       <c r="N44" s="21"/>
     </row>
     <row r="45" spans="1:15" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A45" s="79"/>
-      <c r="B45" s="62"/>
-      <c r="C45" s="63"/>
-      <c r="D45" s="64" t="s">
+      <c r="A45" s="70"/>
+      <c r="B45" s="86"/>
+      <c r="C45" s="87"/>
+      <c r="D45" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="E45" s="65"/>
-      <c r="F45" s="68"/>
-      <c r="G45" s="41"/>
+      <c r="E45" s="44"/>
+      <c r="F45" s="80"/>
+      <c r="G45" s="82"/>
       <c r="H45" s="23"/>
       <c r="I45" s="23"/>
       <c r="J45" s="23"/>
@@ -7164,111 +7172,111 @@
       <c r="N45" s="21"/>
     </row>
     <row r="46" spans="1:15" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A46" s="79"/>
-      <c r="B46" s="58" t="s">
+      <c r="A46" s="70"/>
+      <c r="B46" s="84" t="s">
         <v>65</v>
       </c>
-      <c r="C46" s="59"/>
-      <c r="D46" s="64" t="s">
+      <c r="C46" s="85"/>
+      <c r="D46" s="43" t="s">
         <v>66</v>
       </c>
-      <c r="E46" s="65"/>
-      <c r="F46" s="66">
+      <c r="E46" s="44"/>
+      <c r="F46" s="78">
         <v>0</v>
       </c>
-      <c r="G46" s="41"/>
+      <c r="G46" s="82"/>
       <c r="K46" s="21"/>
       <c r="L46" s="21"/>
       <c r="M46" s="21"/>
       <c r="N46" s="21"/>
     </row>
     <row r="47" spans="1:15" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A47" s="79"/>
-      <c r="B47" s="60"/>
-      <c r="C47" s="61"/>
-      <c r="D47" s="64" t="s">
+      <c r="A47" s="70"/>
+      <c r="B47" s="88"/>
+      <c r="C47" s="89"/>
+      <c r="D47" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="E47" s="65"/>
-      <c r="F47" s="67"/>
-      <c r="G47" s="41"/>
+      <c r="E47" s="44"/>
+      <c r="F47" s="79"/>
+      <c r="G47" s="82"/>
       <c r="K47" s="21"/>
       <c r="L47" s="21"/>
       <c r="M47" s="21"/>
       <c r="N47" s="21"/>
     </row>
     <row r="48" spans="1:15" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A48" s="79"/>
-      <c r="B48" s="60"/>
-      <c r="C48" s="61"/>
-      <c r="D48" s="64" t="s">
+      <c r="A48" s="70"/>
+      <c r="B48" s="88"/>
+      <c r="C48" s="89"/>
+      <c r="D48" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="E48" s="65"/>
-      <c r="F48" s="67"/>
-      <c r="G48" s="41"/>
+      <c r="E48" s="44"/>
+      <c r="F48" s="79"/>
+      <c r="G48" s="82"/>
       <c r="K48" s="21"/>
       <c r="L48" s="21"/>
       <c r="M48" s="21"/>
       <c r="N48" s="21"/>
     </row>
     <row r="49" spans="1:16" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A49" s="79"/>
-      <c r="B49" s="60"/>
-      <c r="C49" s="61"/>
-      <c r="D49" s="64" t="s">
+      <c r="A49" s="70"/>
+      <c r="B49" s="88"/>
+      <c r="C49" s="89"/>
+      <c r="D49" s="43" t="s">
         <v>69</v>
       </c>
-      <c r="E49" s="65"/>
-      <c r="F49" s="67"/>
-      <c r="G49" s="41"/>
+      <c r="E49" s="44"/>
+      <c r="F49" s="79"/>
+      <c r="G49" s="82"/>
       <c r="K49" s="21"/>
       <c r="L49" s="21"/>
       <c r="M49" s="21"/>
       <c r="N49" s="21"/>
     </row>
     <row r="50" spans="1:16" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A50" s="79"/>
-      <c r="B50" s="60"/>
-      <c r="C50" s="61"/>
-      <c r="D50" s="64" t="s">
+      <c r="A50" s="70"/>
+      <c r="B50" s="88"/>
+      <c r="C50" s="89"/>
+      <c r="D50" s="43" t="s">
         <v>70</v>
       </c>
-      <c r="E50" s="65"/>
-      <c r="F50" s="67"/>
-      <c r="G50" s="41"/>
+      <c r="E50" s="44"/>
+      <c r="F50" s="79"/>
+      <c r="G50" s="82"/>
       <c r="K50" s="21"/>
       <c r="L50" s="21"/>
       <c r="M50" s="21"/>
       <c r="N50" s="21"/>
     </row>
     <row r="51" spans="1:16" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A51" s="80"/>
-      <c r="B51" s="62"/>
-      <c r="C51" s="63"/>
-      <c r="D51" s="64" t="s">
+      <c r="A51" s="71"/>
+      <c r="B51" s="86"/>
+      <c r="C51" s="87"/>
+      <c r="D51" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="E51" s="65"/>
-      <c r="F51" s="68"/>
-      <c r="G51" s="42"/>
+      <c r="E51" s="44"/>
+      <c r="F51" s="80"/>
+      <c r="G51" s="83"/>
       <c r="K51" s="21"/>
       <c r="L51" s="21"/>
       <c r="M51" s="21"/>
       <c r="N51" s="21"/>
     </row>
     <row r="52" spans="1:16" s="8" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A52" s="49" t="s">
+      <c r="A52" s="90" t="s">
         <v>72</v>
       </c>
-      <c r="B52" s="50" t="s">
+      <c r="B52" s="91" t="s">
         <v>73</v>
       </c>
-      <c r="C52" s="50"/>
-      <c r="D52" s="50" t="s">
+      <c r="C52" s="91"/>
+      <c r="D52" s="91" t="s">
         <v>74</v>
       </c>
-      <c r="E52" s="50"/>
+      <c r="E52" s="91"/>
       <c r="F52" s="17">
         <v>0</v>
       </c>
@@ -7280,15 +7288,15 @@
       <c r="M52" s="20"/>
     </row>
     <row r="53" spans="1:16" s="8" customFormat="1" ht="95.25" customHeight="1">
-      <c r="A53" s="49"/>
-      <c r="B53" s="51" t="s">
+      <c r="A53" s="90"/>
+      <c r="B53" s="92" t="s">
         <v>76</v>
       </c>
-      <c r="C53" s="51"/>
-      <c r="D53" s="47" t="s">
+      <c r="C53" s="92"/>
+      <c r="D53" s="93" t="s">
         <v>77</v>
       </c>
-      <c r="E53" s="47"/>
+      <c r="E53" s="93"/>
       <c r="F53" s="26">
         <v>0</v>
       </c>
@@ -7300,19 +7308,19 @@
       <c r="M53" s="20"/>
     </row>
     <row r="54" spans="1:16" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A54" s="49"/>
-      <c r="B54" s="52" t="s">
+      <c r="A54" s="90"/>
+      <c r="B54" s="94" t="s">
         <v>78</v>
       </c>
-      <c r="C54" s="53"/>
-      <c r="D54" s="43" t="s">
+      <c r="C54" s="95"/>
+      <c r="D54" s="100" t="s">
         <v>79</v>
       </c>
-      <c r="E54" s="44"/>
-      <c r="F54" s="37">
+      <c r="E54" s="101"/>
+      <c r="F54" s="103">
         <v>0</v>
       </c>
-      <c r="G54" s="40" t="s">
+      <c r="G54" s="81" t="s">
         <v>80</v>
       </c>
       <c r="K54" s="4"/>
@@ -7321,30 +7329,30 @@
       <c r="N54" s="4"/>
     </row>
     <row r="55" spans="1:16" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A55" s="49"/>
-      <c r="B55" s="54"/>
-      <c r="C55" s="55"/>
-      <c r="D55" s="43" t="s">
+      <c r="A55" s="90"/>
+      <c r="B55" s="96"/>
+      <c r="C55" s="97"/>
+      <c r="D55" s="100" t="s">
         <v>81</v>
       </c>
-      <c r="E55" s="44"/>
-      <c r="F55" s="38"/>
-      <c r="G55" s="41"/>
+      <c r="E55" s="101"/>
+      <c r="F55" s="104"/>
+      <c r="G55" s="82"/>
       <c r="K55" s="4"/>
       <c r="L55" s="4"/>
       <c r="M55" s="4"/>
       <c r="N55" s="4"/>
     </row>
     <row r="56" spans="1:16" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A56" s="49"/>
-      <c r="B56" s="54"/>
-      <c r="C56" s="55"/>
-      <c r="D56" s="43" t="s">
+      <c r="A56" s="90"/>
+      <c r="B56" s="96"/>
+      <c r="C56" s="97"/>
+      <c r="D56" s="100" t="s">
         <v>82</v>
       </c>
-      <c r="E56" s="44"/>
-      <c r="F56" s="38"/>
-      <c r="G56" s="41"/>
+      <c r="E56" s="101"/>
+      <c r="F56" s="104"/>
+      <c r="G56" s="82"/>
       <c r="J56" s="4"/>
       <c r="K56" s="4"/>
       <c r="L56" s="4"/>
@@ -7352,15 +7360,15 @@
       <c r="N56" s="4"/>
     </row>
     <row r="57" spans="1:16" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A57" s="49"/>
-      <c r="B57" s="56"/>
-      <c r="C57" s="57"/>
-      <c r="D57" s="43" t="s">
+      <c r="A57" s="90"/>
+      <c r="B57" s="98"/>
+      <c r="C57" s="99"/>
+      <c r="D57" s="100" t="s">
         <v>83</v>
       </c>
-      <c r="E57" s="44"/>
-      <c r="F57" s="39"/>
-      <c r="G57" s="42"/>
+      <c r="E57" s="101"/>
+      <c r="F57" s="105"/>
+      <c r="G57" s="83"/>
       <c r="H57" s="1"/>
       <c r="I57" s="1"/>
       <c r="J57" s="3"/>
@@ -7370,19 +7378,19 @@
       <c r="N57" s="3"/>
     </row>
     <row r="58" spans="1:16" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A58" s="49"/>
-      <c r="B58" s="45" t="s">
+      <c r="A58" s="90"/>
+      <c r="B58" s="102" t="s">
         <v>84</v>
       </c>
-      <c r="C58" s="45"/>
-      <c r="D58" s="45" t="s">
+      <c r="C58" s="102"/>
+      <c r="D58" s="102" t="s">
         <v>85</v>
       </c>
-      <c r="E58" s="45"/>
-      <c r="F58" s="46">
+      <c r="E58" s="102"/>
+      <c r="F58" s="106">
         <v>0</v>
       </c>
-      <c r="G58" s="47" t="s">
+      <c r="G58" s="93" t="s">
         <v>86</v>
       </c>
       <c r="K58" s="4"/>
@@ -7391,44 +7399,44 @@
       <c r="N58" s="4"/>
     </row>
     <row r="59" spans="1:16" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A59" s="49"/>
-      <c r="B59" s="45"/>
-      <c r="C59" s="45"/>
-      <c r="D59" s="48" t="s">
+      <c r="A59" s="90"/>
+      <c r="B59" s="102"/>
+      <c r="C59" s="102"/>
+      <c r="D59" s="107" t="s">
         <v>87</v>
       </c>
-      <c r="E59" s="48"/>
-      <c r="F59" s="46"/>
-      <c r="G59" s="47"/>
+      <c r="E59" s="107"/>
+      <c r="F59" s="106"/>
+      <c r="G59" s="93"/>
       <c r="K59" s="4"/>
       <c r="L59" s="4"/>
       <c r="M59" s="4"/>
       <c r="N59" s="4"/>
     </row>
     <row r="60" spans="1:16" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A60" s="49"/>
-      <c r="B60" s="45"/>
-      <c r="C60" s="45"/>
-      <c r="D60" s="45" t="s">
+      <c r="A60" s="90"/>
+      <c r="B60" s="102"/>
+      <c r="C60" s="102"/>
+      <c r="D60" s="102" t="s">
         <v>88</v>
       </c>
-      <c r="E60" s="45"/>
-      <c r="F60" s="46"/>
-      <c r="G60" s="47"/>
+      <c r="E60" s="102"/>
+      <c r="F60" s="106"/>
+      <c r="G60" s="93"/>
       <c r="K60" s="4"/>
       <c r="L60" s="4"/>
       <c r="M60" s="4"/>
     </row>
     <row r="61" spans="1:16" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A61" s="49"/>
-      <c r="B61" s="45"/>
-      <c r="C61" s="45"/>
-      <c r="D61" s="45" t="s">
+      <c r="A61" s="90"/>
+      <c r="B61" s="102"/>
+      <c r="C61" s="102"/>
+      <c r="D61" s="102" t="s">
         <v>89</v>
       </c>
-      <c r="E61" s="45"/>
-      <c r="F61" s="46"/>
-      <c r="G61" s="47"/>
+      <c r="E61" s="102"/>
+      <c r="F61" s="106"/>
+      <c r="G61" s="93"/>
       <c r="K61" s="4"/>
       <c r="L61" s="4"/>
       <c r="M61" s="4"/>
@@ -7446,50 +7454,39 @@
     </row>
   </sheetData>
   <mergeCells count="101">
-    <mergeCell ref="F54:F57"/>
-    <mergeCell ref="G54:G57"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="B58:C61"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="F58:F61"/>
-    <mergeCell ref="G58:G61"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="A52:A61"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="B54:C57"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="B44:C45"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="F44:F45"/>
-    <mergeCell ref="G44:G51"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="B46:C51"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="F46:F51"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="G42:G43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="G32:G41"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="B37:C41"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="F37:F41"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="A7:G7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="A9:A51"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="F15:F19"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="B10:C14"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:F14"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="B32:C36"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="F32:F36"/>
+    <mergeCell ref="B22:C26"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:F26"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="B42:C43"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:F43"/>
     <mergeCell ref="G10:G19"/>
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="D12:E12"/>
@@ -7514,39 +7511,50 @@
     <mergeCell ref="D28:E28"/>
     <mergeCell ref="D29:E29"/>
     <mergeCell ref="D30:E30"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="A9:A51"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="F15:F19"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="B10:C14"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:F14"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="B32:C36"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="F32:F36"/>
-    <mergeCell ref="B22:C26"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:F26"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="B42:C43"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:F43"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="C6:G6"/>
-    <mergeCell ref="A7:G7"/>
+    <mergeCell ref="G42:G43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="G32:G41"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="B37:C41"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="F37:F41"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="B44:C45"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="F44:F45"/>
+    <mergeCell ref="G44:G51"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="B46:C51"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="F46:F51"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="A52:A61"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="B54:C57"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="F54:F57"/>
+    <mergeCell ref="G54:G57"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="B58:C61"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="F58:F61"/>
+    <mergeCell ref="G58:G61"/>
+    <mergeCell ref="D59:E59"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="F52">

</xml_diff>

<commit_message>
template beans to excel
</commit_message>
<xml_diff>
--- a/src/test/resources/hanergy-ceping.xlsx
+++ b/src/test/resources/hanergy-ceping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bingoo/GitHub/excel2javabeans/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41A78A56-E419-8048-AA4C-AABCD3130A5F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21E6A36B-BDF6-EC40-A1BC-D32EF361E1CF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{ED7C35D1-08C2-1B4F-A1CE-BB55E02E4662}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{ED7C35D1-08C2-1B4F-A1CE-BB55E02E4662}"/>
   </bookViews>
   <sheets>
     <sheet name="有评语-模板" sheetId="5" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="95">
   <si>
     <t>大数据类候选人测评结论表</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -448,6 +448,10 @@
     <t>高潜（均值≥5.26）
 (一票否决)</t>
     <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>文化</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -769,7 +773,7 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -900,12 +904,57 @@
     <xf numFmtId="0" fontId="13" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -921,6 +970,150 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="10" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -930,177 +1123,6 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="10" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="10" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="10" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="10" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1118,9 +1140,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -4848,7 +4867,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="107" zoomScaleSheetLayoutView="125" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="17"/>
@@ -4864,36 +4883,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="32.25" customHeight="1">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
     </row>
     <row r="3" spans="1:7" s="8" customFormat="1" ht="27" customHeight="1">
       <c r="A3" s="34" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="34"/>
-      <c r="C3" s="45" t="s">
+      <c r="C3" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="45"/>
+      <c r="D3" s="54"/>
       <c r="E3" s="6"/>
       <c r="F3" s="34" t="s">
         <v>4</v>
@@ -4905,10 +4924,10 @@
         <v>5</v>
       </c>
       <c r="B4" s="34"/>
-      <c r="C4" s="45" t="s">
+      <c r="C4" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="45"/>
+      <c r="D4" s="54"/>
       <c r="E4" s="10"/>
       <c r="F4" s="32" t="s">
         <v>7</v>
@@ -4919,25 +4938,25 @@
       <c r="A5" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="106" t="s">
+      <c r="B5" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="45">
+      <c r="C5" s="54">
         <v>1.2</v>
       </c>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="54"/>
+      <c r="F5" s="54"/>
+      <c r="G5" s="54"/>
     </row>
     <row r="6" spans="1:7" s="13" customFormat="1" ht="48" customHeight="1">
       <c r="A6" s="40"/>
-      <c r="B6" s="106"/>
-      <c r="C6" s="117"/>
-      <c r="D6" s="117"/>
-      <c r="E6" s="117"/>
-      <c r="F6" s="117"/>
-      <c r="G6" s="117"/>
+      <c r="B6" s="55"/>
+      <c r="C6" s="56"/>
+      <c r="D6" s="56"/>
+      <c r="E6" s="56"/>
+      <c r="F6" s="56"/>
+      <c r="G6" s="56"/>
     </row>
     <row r="7" spans="1:7" s="37" customFormat="1" ht="40" customHeight="1">
       <c r="A7" s="40"/>
@@ -4953,28 +4972,28 @@
       <c r="G7" s="41"/>
     </row>
     <row r="8" spans="1:7" s="8" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A8" s="54" t="s">
+      <c r="A8" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="59"/>
-      <c r="C8" s="59"/>
-      <c r="D8" s="59"/>
-      <c r="E8" s="59"/>
-      <c r="F8" s="59"/>
-      <c r="G8" s="55"/>
+      <c r="B8" s="52"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="52"/>
+      <c r="E8" s="52"/>
+      <c r="F8" s="52"/>
+      <c r="G8" s="50"/>
     </row>
     <row r="9" spans="1:7" s="8" customFormat="1" ht="18" customHeight="1">
       <c r="A9" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="54" t="s">
+      <c r="B9" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="55"/>
-      <c r="D9" s="56" t="s">
+      <c r="C9" s="50"/>
+      <c r="D9" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="56"/>
+      <c r="E9" s="51"/>
       <c r="F9" s="33" t="s">
         <v>14</v>
       </c>
@@ -4983,27 +5002,28 @@
       </c>
     </row>
     <row r="10" spans="1:7" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A10" s="32" t="s">
+      <c r="A10" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="43"/>
-      <c r="D10" s="57" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" s="58"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="18" t="s">
+      <c r="C10" s="47"/>
+      <c r="D10" s="45" t="s">
+        <v>94</v>
+      </c>
+      <c r="E10" s="41"/>
+      <c r="F10" s="48">
+        <v>5.8</v>
+      </c>
+      <c r="G10" s="39" t="s">
         <v>19</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="10">
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
     <mergeCell ref="A8:G8"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A2:G2"/>
@@ -5050,15 +5070,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="1" customFormat="1" ht="32.25" customHeight="1">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
       <c r="J1" s="2"/>
       <c r="L1" s="3"/>
       <c r="M1" s="4"/>
@@ -5067,15 +5087,15 @@
       <c r="P1" s="4"/>
     </row>
     <row r="2" spans="1:17" s="1" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
       <c r="J2" s="2"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
@@ -5088,10 +5108,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="34"/>
-      <c r="C3" s="45" t="s">
+      <c r="C3" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="45"/>
+      <c r="D3" s="54"/>
       <c r="E3" s="6"/>
       <c r="F3" s="34" t="s">
         <v>4</v>
@@ -5109,10 +5129,10 @@
         <v>5</v>
       </c>
       <c r="B4" s="34"/>
-      <c r="C4" s="45" t="s">
+      <c r="C4" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="45"/>
+      <c r="D4" s="54"/>
       <c r="E4" s="10"/>
       <c r="F4" s="32" t="s">
         <v>7</v>
@@ -5126,19 +5146,19 @@
       <c r="Q4" s="4"/>
     </row>
     <row r="5" spans="1:17" s="8" customFormat="1" ht="49.5" customHeight="1">
-      <c r="A5" s="60" t="s">
+      <c r="A5" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="46" t="s">
+      <c r="B5" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="48">
+      <c r="C5" s="63">
         <v>6</v>
       </c>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="50"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="64"/>
+      <c r="F5" s="64"/>
+      <c r="G5" s="65"/>
       <c r="H5" s="31"/>
       <c r="J5" s="12"/>
       <c r="K5" s="4"/>
@@ -5150,28 +5170,28 @@
       <c r="Q5" s="4"/>
     </row>
     <row r="6" spans="1:17" s="13" customFormat="1" ht="48" customHeight="1">
-      <c r="A6" s="61"/>
-      <c r="B6" s="47"/>
-      <c r="C6" s="62"/>
-      <c r="D6" s="63"/>
-      <c r="E6" s="63"/>
-      <c r="F6" s="63"/>
-      <c r="G6" s="64"/>
+      <c r="A6" s="60"/>
+      <c r="B6" s="62"/>
+      <c r="C6" s="66"/>
+      <c r="D6" s="67"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="67"/>
+      <c r="G6" s="68"/>
       <c r="I6" s="14"/>
       <c r="J6" s="14"/>
       <c r="K6" s="14"/>
       <c r="L6" s="14"/>
     </row>
     <row r="7" spans="1:17" s="8" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A7" s="54" t="s">
+      <c r="A7" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="59"/>
-      <c r="C7" s="59"/>
-      <c r="D7" s="59"/>
-      <c r="E7" s="59"/>
-      <c r="F7" s="59"/>
-      <c r="G7" s="55"/>
+      <c r="B7" s="52"/>
+      <c r="C7" s="52"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="52"/>
+      <c r="F7" s="52"/>
+      <c r="G7" s="50"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
@@ -5181,14 +5201,14 @@
       <c r="A8" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="54" t="s">
+      <c r="B8" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="55"/>
-      <c r="D8" s="56" t="s">
+      <c r="C8" s="50"/>
+      <c r="D8" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="56"/>
+      <c r="E8" s="51"/>
       <c r="F8" s="33" t="s">
         <v>14</v>
       </c>
@@ -5285,36 +5305,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="32.25" customHeight="1">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
     </row>
     <row r="3" spans="1:7" s="8" customFormat="1" ht="27" customHeight="1">
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="5"/>
-      <c r="C3" s="45" t="s">
+      <c r="C3" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="45"/>
+      <c r="D3" s="54"/>
       <c r="E3" s="6"/>
       <c r="F3" s="5" t="s">
         <v>4</v>
@@ -5326,10 +5346,10 @@
         <v>5</v>
       </c>
       <c r="B4" s="5"/>
-      <c r="C4" s="45" t="s">
+      <c r="C4" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="45"/>
+      <c r="D4" s="54"/>
       <c r="E4" s="10"/>
       <c r="F4" s="25" t="s">
         <v>7</v>
@@ -5337,186 +5357,186 @@
       <c r="G4" s="5"/>
     </row>
     <row r="5" spans="1:7" s="8" customFormat="1" ht="49.5" customHeight="1">
-      <c r="A5" s="60" t="s">
+      <c r="A5" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="46" t="s">
+      <c r="B5" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="48">
+      <c r="C5" s="63">
         <v>1.2</v>
       </c>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="50"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="64"/>
+      <c r="F5" s="64"/>
+      <c r="G5" s="65"/>
     </row>
     <row r="6" spans="1:7" s="13" customFormat="1" ht="48" customHeight="1">
-      <c r="A6" s="61"/>
-      <c r="B6" s="47"/>
-      <c r="C6" s="51"/>
-      <c r="D6" s="52"/>
-      <c r="E6" s="52"/>
-      <c r="F6" s="52"/>
-      <c r="G6" s="53"/>
+      <c r="A6" s="60"/>
+      <c r="B6" s="62"/>
+      <c r="C6" s="114"/>
+      <c r="D6" s="115"/>
+      <c r="E6" s="115"/>
+      <c r="F6" s="115"/>
+      <c r="G6" s="116"/>
     </row>
     <row r="7" spans="1:7" s="13" customFormat="1" ht="40" customHeight="1">
-      <c r="A7" s="61"/>
-      <c r="B7" s="111" t="s">
+      <c r="A7" s="60"/>
+      <c r="B7" s="117" t="s">
         <v>90</v>
       </c>
       <c r="C7" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="D7" s="107"/>
-      <c r="E7" s="107"/>
-      <c r="F7" s="107"/>
-      <c r="G7" s="107"/>
+      <c r="D7" s="110"/>
+      <c r="E7" s="110"/>
+      <c r="F7" s="110"/>
+      <c r="G7" s="110"/>
     </row>
     <row r="8" spans="1:7" s="13" customFormat="1" ht="40" customHeight="1">
-      <c r="A8" s="61"/>
-      <c r="B8" s="112"/>
-      <c r="C8" s="106" t="s">
+      <c r="A8" s="60"/>
+      <c r="B8" s="118"/>
+      <c r="C8" s="55" t="s">
         <v>91</v>
       </c>
-      <c r="D8" s="107"/>
-      <c r="E8" s="107"/>
-      <c r="F8" s="107"/>
-      <c r="G8" s="107"/>
+      <c r="D8" s="110"/>
+      <c r="E8" s="110"/>
+      <c r="F8" s="110"/>
+      <c r="G8" s="110"/>
     </row>
     <row r="9" spans="1:7" s="13" customFormat="1" ht="40" customHeight="1">
-      <c r="A9" s="61"/>
-      <c r="B9" s="112"/>
-      <c r="C9" s="106"/>
-      <c r="D9" s="107"/>
-      <c r="E9" s="107"/>
-      <c r="F9" s="107"/>
-      <c r="G9" s="107"/>
+      <c r="A9" s="60"/>
+      <c r="B9" s="118"/>
+      <c r="C9" s="55"/>
+      <c r="D9" s="110"/>
+      <c r="E9" s="110"/>
+      <c r="F9" s="110"/>
+      <c r="G9" s="110"/>
     </row>
     <row r="10" spans="1:7" s="13" customFormat="1" ht="40" customHeight="1">
-      <c r="A10" s="61"/>
-      <c r="B10" s="112"/>
-      <c r="C10" s="106"/>
-      <c r="D10" s="107"/>
-      <c r="E10" s="107"/>
-      <c r="F10" s="107"/>
-      <c r="G10" s="107"/>
+      <c r="A10" s="60"/>
+      <c r="B10" s="118"/>
+      <c r="C10" s="55"/>
+      <c r="D10" s="110"/>
+      <c r="E10" s="110"/>
+      <c r="F10" s="110"/>
+      <c r="G10" s="110"/>
     </row>
     <row r="11" spans="1:7" s="13" customFormat="1" ht="40" customHeight="1">
-      <c r="A11" s="61"/>
-      <c r="B11" s="112"/>
-      <c r="C11" s="106"/>
-      <c r="D11" s="108"/>
-      <c r="E11" s="109"/>
-      <c r="F11" s="109"/>
-      <c r="G11" s="110"/>
+      <c r="A11" s="60"/>
+      <c r="B11" s="118"/>
+      <c r="C11" s="55"/>
+      <c r="D11" s="111"/>
+      <c r="E11" s="112"/>
+      <c r="F11" s="112"/>
+      <c r="G11" s="113"/>
     </row>
     <row r="12" spans="1:7" s="13" customFormat="1" ht="40" customHeight="1">
-      <c r="A12" s="61"/>
-      <c r="B12" s="112"/>
-      <c r="C12" s="106"/>
-      <c r="D12" s="107"/>
-      <c r="E12" s="107"/>
-      <c r="F12" s="107"/>
-      <c r="G12" s="107"/>
+      <c r="A12" s="60"/>
+      <c r="B12" s="118"/>
+      <c r="C12" s="55"/>
+      <c r="D12" s="110"/>
+      <c r="E12" s="110"/>
+      <c r="F12" s="110"/>
+      <c r="G12" s="110"/>
     </row>
     <row r="13" spans="1:7" s="13" customFormat="1" ht="40" customHeight="1">
-      <c r="A13" s="61"/>
-      <c r="B13" s="112"/>
-      <c r="C13" s="106"/>
-      <c r="D13" s="107"/>
-      <c r="E13" s="107"/>
-      <c r="F13" s="107"/>
-      <c r="G13" s="107"/>
+      <c r="A13" s="60"/>
+      <c r="B13" s="118"/>
+      <c r="C13" s="55"/>
+      <c r="D13" s="110"/>
+      <c r="E13" s="110"/>
+      <c r="F13" s="110"/>
+      <c r="G13" s="110"/>
     </row>
     <row r="14" spans="1:7" s="13" customFormat="1" ht="40" customHeight="1">
-      <c r="A14" s="61"/>
-      <c r="B14" s="112"/>
-      <c r="C14" s="106"/>
-      <c r="D14" s="108"/>
-      <c r="E14" s="109"/>
-      <c r="F14" s="109"/>
-      <c r="G14" s="110"/>
+      <c r="A14" s="60"/>
+      <c r="B14" s="118"/>
+      <c r="C14" s="55"/>
+      <c r="D14" s="111"/>
+      <c r="E14" s="112"/>
+      <c r="F14" s="112"/>
+      <c r="G14" s="113"/>
     </row>
     <row r="15" spans="1:7" s="13" customFormat="1" ht="40" customHeight="1">
-      <c r="A15" s="61"/>
-      <c r="B15" s="112"/>
-      <c r="C15" s="106"/>
-      <c r="D15" s="108"/>
-      <c r="E15" s="109"/>
-      <c r="F15" s="109"/>
-      <c r="G15" s="110"/>
+      <c r="A15" s="60"/>
+      <c r="B15" s="118"/>
+      <c r="C15" s="55"/>
+      <c r="D15" s="111"/>
+      <c r="E15" s="112"/>
+      <c r="F15" s="112"/>
+      <c r="G15" s="113"/>
     </row>
     <row r="16" spans="1:7" s="13" customFormat="1" ht="40" customHeight="1">
-      <c r="A16" s="61"/>
-      <c r="B16" s="112"/>
-      <c r="C16" s="106"/>
-      <c r="D16" s="108"/>
-      <c r="E16" s="109"/>
-      <c r="F16" s="109"/>
-      <c r="G16" s="110"/>
+      <c r="A16" s="60"/>
+      <c r="B16" s="118"/>
+      <c r="C16" s="55"/>
+      <c r="D16" s="111"/>
+      <c r="E16" s="112"/>
+      <c r="F16" s="112"/>
+      <c r="G16" s="113"/>
     </row>
     <row r="17" spans="1:7" s="13" customFormat="1" ht="40" customHeight="1">
-      <c r="A17" s="61"/>
-      <c r="B17" s="112"/>
-      <c r="C17" s="106"/>
-      <c r="D17" s="108"/>
-      <c r="E17" s="109"/>
-      <c r="F17" s="109"/>
-      <c r="G17" s="110"/>
+      <c r="A17" s="60"/>
+      <c r="B17" s="118"/>
+      <c r="C17" s="55"/>
+      <c r="D17" s="111"/>
+      <c r="E17" s="112"/>
+      <c r="F17" s="112"/>
+      <c r="G17" s="113"/>
     </row>
     <row r="18" spans="1:7" s="13" customFormat="1" ht="40" customHeight="1">
-      <c r="A18" s="61"/>
-      <c r="B18" s="112"/>
-      <c r="C18" s="106"/>
-      <c r="D18" s="107"/>
-      <c r="E18" s="107"/>
-      <c r="F18" s="107"/>
-      <c r="G18" s="107"/>
+      <c r="A18" s="60"/>
+      <c r="B18" s="118"/>
+      <c r="C18" s="55"/>
+      <c r="D18" s="110"/>
+      <c r="E18" s="110"/>
+      <c r="F18" s="110"/>
+      <c r="G18" s="110"/>
     </row>
     <row r="19" spans="1:7" s="13" customFormat="1" ht="40" customHeight="1">
-      <c r="A19" s="61"/>
-      <c r="B19" s="112"/>
-      <c r="C19" s="46" t="s">
+      <c r="A19" s="60"/>
+      <c r="B19" s="118"/>
+      <c r="C19" s="61" t="s">
         <v>92</v>
       </c>
-      <c r="D19" s="107"/>
-      <c r="E19" s="107"/>
-      <c r="F19" s="107"/>
-      <c r="G19" s="107"/>
+      <c r="D19" s="110"/>
+      <c r="E19" s="110"/>
+      <c r="F19" s="110"/>
+      <c r="G19" s="110"/>
     </row>
     <row r="20" spans="1:7" s="13" customFormat="1" ht="40" customHeight="1">
-      <c r="A20" s="61"/>
-      <c r="B20" s="112"/>
-      <c r="C20" s="113"/>
-      <c r="D20" s="107"/>
-      <c r="E20" s="107"/>
-      <c r="F20" s="107"/>
-      <c r="G20" s="107"/>
+      <c r="A20" s="60"/>
+      <c r="B20" s="118"/>
+      <c r="C20" s="119"/>
+      <c r="D20" s="110"/>
+      <c r="E20" s="110"/>
+      <c r="F20" s="110"/>
+      <c r="G20" s="110"/>
     </row>
     <row r="21" spans="1:7" s="8" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A21" s="54" t="s">
+      <c r="A21" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="59"/>
-      <c r="C21" s="59"/>
-      <c r="D21" s="59"/>
-      <c r="E21" s="59"/>
-      <c r="F21" s="59"/>
-      <c r="G21" s="55"/>
+      <c r="B21" s="52"/>
+      <c r="C21" s="52"/>
+      <c r="D21" s="52"/>
+      <c r="E21" s="52"/>
+      <c r="F21" s="52"/>
+      <c r="G21" s="50"/>
     </row>
     <row r="22" spans="1:7" s="8" customFormat="1" ht="18" customHeight="1">
       <c r="A22" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="54" t="s">
+      <c r="B22" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="55"/>
-      <c r="D22" s="56" t="s">
+      <c r="C22" s="50"/>
+      <c r="D22" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="E22" s="56"/>
+      <c r="E22" s="51"/>
       <c r="F22" s="16" t="s">
         <v>14</v>
       </c>
@@ -5525,13 +5545,13 @@
       </c>
     </row>
     <row r="23" spans="1:7" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A23" s="101" t="s">
+      <c r="A23" s="105" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="104" t="s">
+      <c r="B23" s="108" t="s">
         <v>17</v>
       </c>
-      <c r="C23" s="105"/>
+      <c r="C23" s="109"/>
       <c r="D23" s="57" t="s">
         <v>18</v>
       </c>
@@ -5542,531 +5562,531 @@
       </c>
     </row>
     <row r="24" spans="1:7" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A24" s="102"/>
-      <c r="B24" s="95" t="s">
+      <c r="A24" s="106"/>
+      <c r="B24" s="99" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="96"/>
+      <c r="C24" s="100"/>
       <c r="D24" s="57" t="s">
         <v>21</v>
       </c>
       <c r="E24" s="58"/>
-      <c r="F24" s="74">
+      <c r="F24" s="78">
         <v>2</v>
       </c>
-      <c r="G24" s="65" t="s">
+      <c r="G24" s="69" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:7" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A25" s="102"/>
-      <c r="B25" s="97"/>
-      <c r="C25" s="98"/>
+      <c r="A25" s="106"/>
+      <c r="B25" s="101"/>
+      <c r="C25" s="102"/>
       <c r="D25" s="57" t="s">
         <v>23</v>
       </c>
       <c r="E25" s="58"/>
-      <c r="F25" s="94"/>
-      <c r="G25" s="66"/>
+      <c r="F25" s="98"/>
+      <c r="G25" s="70"/>
     </row>
     <row r="26" spans="1:7" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A26" s="102"/>
-      <c r="B26" s="97"/>
-      <c r="C26" s="98"/>
+      <c r="A26" s="106"/>
+      <c r="B26" s="101"/>
+      <c r="C26" s="102"/>
       <c r="D26" s="57" t="s">
         <v>24</v>
       </c>
       <c r="E26" s="58"/>
-      <c r="F26" s="94"/>
-      <c r="G26" s="66"/>
+      <c r="F26" s="98"/>
+      <c r="G26" s="70"/>
     </row>
     <row r="27" spans="1:7" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A27" s="102"/>
-      <c r="B27" s="97"/>
-      <c r="C27" s="98"/>
+      <c r="A27" s="106"/>
+      <c r="B27" s="101"/>
+      <c r="C27" s="102"/>
       <c r="D27" s="57" t="s">
         <v>25</v>
       </c>
       <c r="E27" s="58"/>
-      <c r="F27" s="94"/>
-      <c r="G27" s="66"/>
+      <c r="F27" s="98"/>
+      <c r="G27" s="70"/>
     </row>
     <row r="28" spans="1:7" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A28" s="102"/>
-      <c r="B28" s="99"/>
-      <c r="C28" s="100"/>
+      <c r="A28" s="106"/>
+      <c r="B28" s="103"/>
+      <c r="C28" s="104"/>
       <c r="D28" s="57" t="s">
         <v>26</v>
       </c>
       <c r="E28" s="58"/>
-      <c r="F28" s="75"/>
-      <c r="G28" s="66"/>
+      <c r="F28" s="79"/>
+      <c r="G28" s="70"/>
     </row>
     <row r="29" spans="1:7" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A29" s="102"/>
-      <c r="B29" s="88" t="s">
+      <c r="A29" s="106"/>
+      <c r="B29" s="92" t="s">
         <v>27</v>
       </c>
-      <c r="C29" s="89"/>
+      <c r="C29" s="93"/>
       <c r="D29" s="57" t="s">
         <v>28</v>
       </c>
       <c r="E29" s="58"/>
-      <c r="F29" s="74">
+      <c r="F29" s="78">
         <v>2</v>
       </c>
-      <c r="G29" s="66"/>
+      <c r="G29" s="70"/>
     </row>
     <row r="30" spans="1:7" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A30" s="102"/>
-      <c r="B30" s="92"/>
-      <c r="C30" s="93"/>
+      <c r="A30" s="106"/>
+      <c r="B30" s="96"/>
+      <c r="C30" s="97"/>
       <c r="D30" s="57" t="s">
         <v>29</v>
       </c>
       <c r="E30" s="58"/>
-      <c r="F30" s="94"/>
-      <c r="G30" s="66"/>
+      <c r="F30" s="98"/>
+      <c r="G30" s="70"/>
     </row>
     <row r="31" spans="1:7" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A31" s="102"/>
-      <c r="B31" s="92"/>
-      <c r="C31" s="93"/>
+      <c r="A31" s="106"/>
+      <c r="B31" s="96"/>
+      <c r="C31" s="97"/>
       <c r="D31" s="57" t="s">
         <v>30</v>
       </c>
       <c r="E31" s="58"/>
-      <c r="F31" s="94"/>
-      <c r="G31" s="66"/>
+      <c r="F31" s="98"/>
+      <c r="G31" s="70"/>
     </row>
     <row r="32" spans="1:7" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A32" s="102"/>
-      <c r="B32" s="92"/>
-      <c r="C32" s="93"/>
+      <c r="A32" s="106"/>
+      <c r="B32" s="96"/>
+      <c r="C32" s="97"/>
       <c r="D32" s="57" t="s">
         <v>31</v>
       </c>
       <c r="E32" s="58"/>
-      <c r="F32" s="94"/>
-      <c r="G32" s="66"/>
+      <c r="F32" s="98"/>
+      <c r="G32" s="70"/>
     </row>
     <row r="33" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A33" s="102"/>
-      <c r="B33" s="90"/>
-      <c r="C33" s="91"/>
+      <c r="A33" s="106"/>
+      <c r="B33" s="94"/>
+      <c r="C33" s="95"/>
       <c r="D33" s="57" t="s">
         <v>32</v>
       </c>
       <c r="E33" s="58"/>
-      <c r="F33" s="75"/>
-      <c r="G33" s="67"/>
+      <c r="F33" s="79"/>
+      <c r="G33" s="71"/>
     </row>
     <row r="34" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A34" s="102"/>
-      <c r="B34" s="88" t="s">
+      <c r="A34" s="106"/>
+      <c r="B34" s="92" t="s">
         <v>33</v>
       </c>
-      <c r="C34" s="89"/>
+      <c r="C34" s="93"/>
       <c r="D34" s="57" t="s">
         <v>34</v>
       </c>
       <c r="E34" s="58"/>
-      <c r="F34" s="74">
+      <c r="F34" s="78">
         <v>0</v>
       </c>
-      <c r="G34" s="65" t="s">
+      <c r="G34" s="69" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="35" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A35" s="102"/>
-      <c r="B35" s="90"/>
-      <c r="C35" s="91"/>
+      <c r="A35" s="106"/>
+      <c r="B35" s="94"/>
+      <c r="C35" s="95"/>
       <c r="D35" s="57" t="s">
         <v>33</v>
       </c>
       <c r="E35" s="58"/>
-      <c r="F35" s="75"/>
-      <c r="G35" s="67"/>
+      <c r="F35" s="79"/>
+      <c r="G35" s="71"/>
     </row>
     <row r="36" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A36" s="102"/>
-      <c r="B36" s="95" t="s">
+      <c r="A36" s="106"/>
+      <c r="B36" s="99" t="s">
         <v>36</v>
       </c>
-      <c r="C36" s="96"/>
+      <c r="C36" s="100"/>
       <c r="D36" s="57" t="s">
         <v>37</v>
       </c>
       <c r="E36" s="58"/>
-      <c r="F36" s="74">
+      <c r="F36" s="78">
         <v>2</v>
       </c>
-      <c r="G36" s="65" t="s">
+      <c r="G36" s="69" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="37" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A37" s="102"/>
-      <c r="B37" s="97"/>
-      <c r="C37" s="98"/>
+      <c r="A37" s="106"/>
+      <c r="B37" s="101"/>
+      <c r="C37" s="102"/>
       <c r="D37" s="57" t="s">
         <v>38</v>
       </c>
       <c r="E37" s="58"/>
-      <c r="F37" s="94"/>
-      <c r="G37" s="66"/>
+      <c r="F37" s="98"/>
+      <c r="G37" s="70"/>
     </row>
     <row r="38" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A38" s="102"/>
-      <c r="B38" s="97"/>
-      <c r="C38" s="98"/>
+      <c r="A38" s="106"/>
+      <c r="B38" s="101"/>
+      <c r="C38" s="102"/>
       <c r="D38" s="57" t="s">
         <v>39</v>
       </c>
       <c r="E38" s="58"/>
-      <c r="F38" s="94"/>
-      <c r="G38" s="66"/>
+      <c r="F38" s="98"/>
+      <c r="G38" s="70"/>
     </row>
     <row r="39" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A39" s="102"/>
-      <c r="B39" s="97"/>
-      <c r="C39" s="98"/>
+      <c r="A39" s="106"/>
+      <c r="B39" s="101"/>
+      <c r="C39" s="102"/>
       <c r="D39" s="57" t="s">
         <v>40</v>
       </c>
       <c r="E39" s="58"/>
-      <c r="F39" s="94"/>
-      <c r="G39" s="66"/>
+      <c r="F39" s="98"/>
+      <c r="G39" s="70"/>
     </row>
     <row r="40" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A40" s="102"/>
-      <c r="B40" s="99"/>
-      <c r="C40" s="100"/>
+      <c r="A40" s="106"/>
+      <c r="B40" s="103"/>
+      <c r="C40" s="104"/>
       <c r="D40" s="57" t="s">
         <v>41</v>
       </c>
       <c r="E40" s="58"/>
-      <c r="F40" s="75"/>
-      <c r="G40" s="66"/>
+      <c r="F40" s="79"/>
+      <c r="G40" s="70"/>
       <c r="I40" s="4"/>
     </row>
     <row r="41" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A41" s="102"/>
-      <c r="B41" s="88" t="s">
+      <c r="A41" s="106"/>
+      <c r="B41" s="92" t="s">
         <v>42</v>
       </c>
-      <c r="C41" s="89"/>
+      <c r="C41" s="93"/>
       <c r="D41" s="57" t="s">
         <v>43</v>
       </c>
       <c r="E41" s="58"/>
-      <c r="F41" s="74">
+      <c r="F41" s="78">
         <v>2</v>
       </c>
-      <c r="G41" s="66"/>
+      <c r="G41" s="70"/>
     </row>
     <row r="42" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A42" s="102"/>
-      <c r="B42" s="92"/>
-      <c r="C42" s="93"/>
+      <c r="A42" s="106"/>
+      <c r="B42" s="96"/>
+      <c r="C42" s="97"/>
       <c r="D42" s="57" t="s">
         <v>44</v>
       </c>
       <c r="E42" s="58"/>
-      <c r="F42" s="94"/>
-      <c r="G42" s="66"/>
+      <c r="F42" s="98"/>
+      <c r="G42" s="70"/>
     </row>
     <row r="43" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A43" s="102"/>
-      <c r="B43" s="92"/>
-      <c r="C43" s="93"/>
+      <c r="A43" s="106"/>
+      <c r="B43" s="96"/>
+      <c r="C43" s="97"/>
       <c r="D43" s="57" t="s">
         <v>45</v>
       </c>
       <c r="E43" s="58"/>
-      <c r="F43" s="94"/>
-      <c r="G43" s="66"/>
+      <c r="F43" s="98"/>
+      <c r="G43" s="70"/>
     </row>
     <row r="44" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A44" s="102"/>
-      <c r="B44" s="92"/>
-      <c r="C44" s="93"/>
+      <c r="A44" s="106"/>
+      <c r="B44" s="96"/>
+      <c r="C44" s="97"/>
       <c r="D44" s="57" t="s">
         <v>46</v>
       </c>
       <c r="E44" s="58"/>
-      <c r="F44" s="94"/>
-      <c r="G44" s="66"/>
+      <c r="F44" s="98"/>
+      <c r="G44" s="70"/>
     </row>
     <row r="45" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A45" s="102"/>
-      <c r="B45" s="90"/>
-      <c r="C45" s="91"/>
+      <c r="A45" s="106"/>
+      <c r="B45" s="94"/>
+      <c r="C45" s="95"/>
       <c r="D45" s="57" t="s">
         <v>47</v>
       </c>
       <c r="E45" s="58"/>
-      <c r="F45" s="75"/>
-      <c r="G45" s="66"/>
+      <c r="F45" s="79"/>
+      <c r="G45" s="70"/>
     </row>
     <row r="46" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A46" s="102"/>
-      <c r="B46" s="88" t="s">
+      <c r="A46" s="106"/>
+      <c r="B46" s="92" t="s">
         <v>48</v>
       </c>
-      <c r="C46" s="89"/>
+      <c r="C46" s="93"/>
       <c r="D46" s="57" t="s">
         <v>49</v>
       </c>
       <c r="E46" s="58"/>
-      <c r="F46" s="74">
+      <c r="F46" s="78">
         <v>2</v>
       </c>
-      <c r="G46" s="66"/>
+      <c r="G46" s="70"/>
     </row>
     <row r="47" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A47" s="102"/>
-      <c r="B47" s="92"/>
-      <c r="C47" s="93"/>
+      <c r="A47" s="106"/>
+      <c r="B47" s="96"/>
+      <c r="C47" s="97"/>
       <c r="D47" s="57" t="s">
         <v>51</v>
       </c>
       <c r="E47" s="58"/>
-      <c r="F47" s="94"/>
-      <c r="G47" s="66"/>
+      <c r="F47" s="98"/>
+      <c r="G47" s="70"/>
     </row>
     <row r="48" spans="1:9" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A48" s="102"/>
-      <c r="B48" s="92"/>
-      <c r="C48" s="93"/>
+      <c r="A48" s="106"/>
+      <c r="B48" s="96"/>
+      <c r="C48" s="97"/>
       <c r="D48" s="57" t="s">
         <v>52</v>
       </c>
       <c r="E48" s="58"/>
-      <c r="F48" s="94"/>
-      <c r="G48" s="66"/>
+      <c r="F48" s="98"/>
+      <c r="G48" s="70"/>
     </row>
     <row r="49" spans="1:8" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A49" s="102"/>
-      <c r="B49" s="92"/>
-      <c r="C49" s="93"/>
+      <c r="A49" s="106"/>
+      <c r="B49" s="96"/>
+      <c r="C49" s="97"/>
       <c r="D49" s="57" t="s">
         <v>53</v>
       </c>
       <c r="E49" s="58"/>
-      <c r="F49" s="94"/>
-      <c r="G49" s="66"/>
+      <c r="F49" s="98"/>
+      <c r="G49" s="70"/>
     </row>
     <row r="50" spans="1:8" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A50" s="102"/>
-      <c r="B50" s="90"/>
-      <c r="C50" s="91"/>
+      <c r="A50" s="106"/>
+      <c r="B50" s="94"/>
+      <c r="C50" s="95"/>
       <c r="D50" s="57" t="s">
         <v>54</v>
       </c>
       <c r="E50" s="58"/>
-      <c r="F50" s="75"/>
-      <c r="G50" s="66"/>
+      <c r="F50" s="79"/>
+      <c r="G50" s="70"/>
     </row>
     <row r="51" spans="1:8" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A51" s="102"/>
-      <c r="B51" s="88" t="s">
+      <c r="A51" s="106"/>
+      <c r="B51" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="C51" s="89"/>
+      <c r="C51" s="93"/>
       <c r="D51" s="57" t="s">
         <v>56</v>
       </c>
       <c r="E51" s="58"/>
-      <c r="F51" s="74">
+      <c r="F51" s="78">
         <v>2</v>
       </c>
-      <c r="G51" s="66"/>
+      <c r="G51" s="70"/>
     </row>
     <row r="52" spans="1:8" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A52" s="102"/>
-      <c r="B52" s="92"/>
-      <c r="C52" s="93"/>
+      <c r="A52" s="106"/>
+      <c r="B52" s="96"/>
+      <c r="C52" s="97"/>
       <c r="D52" s="57" t="s">
         <v>23</v>
       </c>
       <c r="E52" s="58"/>
-      <c r="F52" s="94"/>
-      <c r="G52" s="66"/>
+      <c r="F52" s="98"/>
+      <c r="G52" s="70"/>
     </row>
     <row r="53" spans="1:8" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A53" s="102"/>
-      <c r="B53" s="92"/>
-      <c r="C53" s="93"/>
+      <c r="A53" s="106"/>
+      <c r="B53" s="96"/>
+      <c r="C53" s="97"/>
       <c r="D53" s="57" t="s">
         <v>41</v>
       </c>
       <c r="E53" s="58"/>
-      <c r="F53" s="94"/>
-      <c r="G53" s="66"/>
+      <c r="F53" s="98"/>
+      <c r="G53" s="70"/>
     </row>
     <row r="54" spans="1:8" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A54" s="102"/>
-      <c r="B54" s="92"/>
-      <c r="C54" s="93"/>
+      <c r="A54" s="106"/>
+      <c r="B54" s="96"/>
+      <c r="C54" s="97"/>
       <c r="D54" s="57" t="s">
         <v>57</v>
       </c>
       <c r="E54" s="58"/>
-      <c r="F54" s="94"/>
-      <c r="G54" s="66"/>
+      <c r="F54" s="98"/>
+      <c r="G54" s="70"/>
     </row>
     <row r="55" spans="1:8" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A55" s="102"/>
-      <c r="B55" s="90"/>
-      <c r="C55" s="91"/>
+      <c r="A55" s="106"/>
+      <c r="B55" s="94"/>
+      <c r="C55" s="95"/>
       <c r="D55" s="57" t="s">
         <v>58</v>
       </c>
       <c r="E55" s="58"/>
-      <c r="F55" s="75"/>
-      <c r="G55" s="67"/>
+      <c r="F55" s="79"/>
+      <c r="G55" s="71"/>
     </row>
     <row r="56" spans="1:8" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A56" s="102"/>
-      <c r="B56" s="88" t="s">
+      <c r="A56" s="106"/>
+      <c r="B56" s="92" t="s">
         <v>59</v>
       </c>
-      <c r="C56" s="89"/>
+      <c r="C56" s="93"/>
       <c r="D56" s="57" t="s">
         <v>60</v>
       </c>
       <c r="E56" s="58"/>
-      <c r="F56" s="74">
+      <c r="F56" s="78">
         <v>0</v>
       </c>
-      <c r="G56" s="65" t="s">
+      <c r="G56" s="69" t="s">
         <v>35</v>
       </c>
       <c r="H56" s="8"/>
     </row>
     <row r="57" spans="1:8" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A57" s="102"/>
-      <c r="B57" s="90"/>
-      <c r="C57" s="91"/>
+      <c r="A57" s="106"/>
+      <c r="B57" s="94"/>
+      <c r="C57" s="95"/>
       <c r="D57" s="57" t="s">
         <v>61</v>
       </c>
       <c r="E57" s="58"/>
-      <c r="F57" s="75"/>
-      <c r="G57" s="67"/>
+      <c r="F57" s="79"/>
+      <c r="G57" s="71"/>
     </row>
     <row r="58" spans="1:8" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A58" s="102"/>
-      <c r="B58" s="88" t="s">
+      <c r="A58" s="106"/>
+      <c r="B58" s="92" t="s">
         <v>62</v>
       </c>
-      <c r="C58" s="89"/>
+      <c r="C58" s="93"/>
       <c r="D58" s="57" t="s">
         <v>63</v>
       </c>
       <c r="E58" s="58"/>
-      <c r="F58" s="74">
+      <c r="F58" s="78">
         <v>0</v>
       </c>
-      <c r="G58" s="65" t="s">
+      <c r="G58" s="69" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="59" spans="1:8" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A59" s="102"/>
-      <c r="B59" s="90"/>
-      <c r="C59" s="91"/>
+      <c r="A59" s="106"/>
+      <c r="B59" s="94"/>
+      <c r="C59" s="95"/>
       <c r="D59" s="57" t="s">
         <v>64</v>
       </c>
       <c r="E59" s="58"/>
-      <c r="F59" s="75"/>
-      <c r="G59" s="66"/>
+      <c r="F59" s="79"/>
+      <c r="G59" s="70"/>
     </row>
     <row r="60" spans="1:8" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A60" s="102"/>
-      <c r="B60" s="88" t="s">
+      <c r="A60" s="106"/>
+      <c r="B60" s="92" t="s">
         <v>65</v>
       </c>
-      <c r="C60" s="89"/>
+      <c r="C60" s="93"/>
       <c r="D60" s="57" t="s">
         <v>66</v>
       </c>
       <c r="E60" s="58"/>
-      <c r="F60" s="74">
+      <c r="F60" s="78">
         <v>0</v>
       </c>
-      <c r="G60" s="66"/>
+      <c r="G60" s="70"/>
     </row>
     <row r="61" spans="1:8" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A61" s="102"/>
-      <c r="B61" s="92"/>
-      <c r="C61" s="93"/>
+      <c r="A61" s="106"/>
+      <c r="B61" s="96"/>
+      <c r="C61" s="97"/>
       <c r="D61" s="57" t="s">
         <v>67</v>
       </c>
       <c r="E61" s="58"/>
-      <c r="F61" s="94"/>
-      <c r="G61" s="66"/>
+      <c r="F61" s="98"/>
+      <c r="G61" s="70"/>
     </row>
     <row r="62" spans="1:8" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A62" s="102"/>
-      <c r="B62" s="92"/>
-      <c r="C62" s="93"/>
+      <c r="A62" s="106"/>
+      <c r="B62" s="96"/>
+      <c r="C62" s="97"/>
       <c r="D62" s="57" t="s">
         <v>68</v>
       </c>
       <c r="E62" s="58"/>
-      <c r="F62" s="94"/>
-      <c r="G62" s="66"/>
+      <c r="F62" s="98"/>
+      <c r="G62" s="70"/>
     </row>
     <row r="63" spans="1:8" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A63" s="102"/>
-      <c r="B63" s="92"/>
-      <c r="C63" s="93"/>
+      <c r="A63" s="106"/>
+      <c r="B63" s="96"/>
+      <c r="C63" s="97"/>
       <c r="D63" s="57" t="s">
         <v>69</v>
       </c>
       <c r="E63" s="58"/>
-      <c r="F63" s="94"/>
-      <c r="G63" s="66"/>
+      <c r="F63" s="98"/>
+      <c r="G63" s="70"/>
     </row>
     <row r="64" spans="1:8" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A64" s="102"/>
-      <c r="B64" s="92"/>
-      <c r="C64" s="93"/>
+      <c r="A64" s="106"/>
+      <c r="B64" s="96"/>
+      <c r="C64" s="97"/>
       <c r="D64" s="57" t="s">
         <v>70</v>
       </c>
       <c r="E64" s="58"/>
-      <c r="F64" s="94"/>
-      <c r="G64" s="66"/>
+      <c r="F64" s="98"/>
+      <c r="G64" s="70"/>
     </row>
     <row r="65" spans="1:7" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A65" s="103"/>
-      <c r="B65" s="90"/>
-      <c r="C65" s="91"/>
+      <c r="A65" s="107"/>
+      <c r="B65" s="94"/>
+      <c r="C65" s="95"/>
       <c r="D65" s="57" t="s">
         <v>71</v>
       </c>
       <c r="E65" s="58"/>
-      <c r="F65" s="75"/>
-      <c r="G65" s="67"/>
+      <c r="F65" s="79"/>
+      <c r="G65" s="71"/>
     </row>
     <row r="66" spans="1:7" s="8" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A66" s="76" t="s">
+      <c r="A66" s="80" t="s">
         <v>72</v>
       </c>
-      <c r="B66" s="77" t="s">
+      <c r="B66" s="81" t="s">
         <v>73</v>
       </c>
-      <c r="C66" s="77"/>
-      <c r="D66" s="77" t="s">
+      <c r="C66" s="81"/>
+      <c r="D66" s="81" t="s">
         <v>74</v>
       </c>
-      <c r="E66" s="77"/>
+      <c r="E66" s="81"/>
       <c r="F66" s="17">
         <v>0</v>
       </c>
@@ -6075,15 +6095,15 @@
       </c>
     </row>
     <row r="67" spans="1:7" s="8" customFormat="1" ht="95.25" customHeight="1">
-      <c r="A67" s="76"/>
-      <c r="B67" s="78" t="s">
+      <c r="A67" s="80"/>
+      <c r="B67" s="82" t="s">
         <v>76</v>
       </c>
-      <c r="C67" s="78"/>
-      <c r="D67" s="72" t="s">
+      <c r="C67" s="82"/>
+      <c r="D67" s="76" t="s">
         <v>77</v>
       </c>
-      <c r="E67" s="72"/>
+      <c r="E67" s="76"/>
       <c r="F67" s="26">
         <v>0</v>
       </c>
@@ -6092,104 +6112,104 @@
       </c>
     </row>
     <row r="68" spans="1:7" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A68" s="76"/>
-      <c r="B68" s="79" t="s">
+      <c r="A68" s="80"/>
+      <c r="B68" s="83" t="s">
         <v>78</v>
       </c>
-      <c r="C68" s="80"/>
-      <c r="D68" s="68" t="s">
+      <c r="C68" s="84"/>
+      <c r="D68" s="72" t="s">
         <v>79</v>
       </c>
-      <c r="E68" s="69"/>
-      <c r="F68" s="85">
+      <c r="E68" s="73"/>
+      <c r="F68" s="89">
         <v>0</v>
       </c>
-      <c r="G68" s="65" t="s">
+      <c r="G68" s="69" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="69" spans="1:7" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A69" s="76"/>
-      <c r="B69" s="81"/>
-      <c r="C69" s="82"/>
-      <c r="D69" s="68" t="s">
+      <c r="A69" s="80"/>
+      <c r="B69" s="85"/>
+      <c r="C69" s="86"/>
+      <c r="D69" s="72" t="s">
         <v>81</v>
       </c>
-      <c r="E69" s="69"/>
-      <c r="F69" s="86"/>
-      <c r="G69" s="66"/>
+      <c r="E69" s="73"/>
+      <c r="F69" s="90"/>
+      <c r="G69" s="70"/>
     </row>
     <row r="70" spans="1:7" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A70" s="76"/>
-      <c r="B70" s="81"/>
-      <c r="C70" s="82"/>
-      <c r="D70" s="68" t="s">
+      <c r="A70" s="80"/>
+      <c r="B70" s="85"/>
+      <c r="C70" s="86"/>
+      <c r="D70" s="72" t="s">
         <v>82</v>
       </c>
-      <c r="E70" s="69"/>
-      <c r="F70" s="86"/>
-      <c r="G70" s="66"/>
+      <c r="E70" s="73"/>
+      <c r="F70" s="90"/>
+      <c r="G70" s="70"/>
     </row>
     <row r="71" spans="1:7" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A71" s="76"/>
-      <c r="B71" s="83"/>
-      <c r="C71" s="84"/>
-      <c r="D71" s="68" t="s">
+      <c r="A71" s="80"/>
+      <c r="B71" s="87"/>
+      <c r="C71" s="88"/>
+      <c r="D71" s="72" t="s">
         <v>83</v>
       </c>
-      <c r="E71" s="69"/>
-      <c r="F71" s="87"/>
-      <c r="G71" s="67"/>
+      <c r="E71" s="73"/>
+      <c r="F71" s="91"/>
+      <c r="G71" s="71"/>
     </row>
     <row r="72" spans="1:7" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A72" s="76"/>
-      <c r="B72" s="70" t="s">
+      <c r="A72" s="80"/>
+      <c r="B72" s="74" t="s">
         <v>84</v>
       </c>
-      <c r="C72" s="70"/>
-      <c r="D72" s="70" t="s">
+      <c r="C72" s="74"/>
+      <c r="D72" s="74" t="s">
         <v>85</v>
       </c>
-      <c r="E72" s="70"/>
-      <c r="F72" s="71">
+      <c r="E72" s="74"/>
+      <c r="F72" s="75">
         <v>0</v>
       </c>
-      <c r="G72" s="72" t="s">
+      <c r="G72" s="76" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="73" spans="1:7" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A73" s="76"/>
-      <c r="B73" s="70"/>
-      <c r="C73" s="70"/>
-      <c r="D73" s="73" t="s">
+      <c r="A73" s="80"/>
+      <c r="B73" s="74"/>
+      <c r="C73" s="74"/>
+      <c r="D73" s="77" t="s">
         <v>87</v>
       </c>
-      <c r="E73" s="73"/>
-      <c r="F73" s="71"/>
-      <c r="G73" s="72"/>
+      <c r="E73" s="77"/>
+      <c r="F73" s="75"/>
+      <c r="G73" s="76"/>
     </row>
     <row r="74" spans="1:7" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A74" s="76"/>
-      <c r="B74" s="70"/>
-      <c r="C74" s="70"/>
-      <c r="D74" s="70" t="s">
+      <c r="A74" s="80"/>
+      <c r="B74" s="74"/>
+      <c r="C74" s="74"/>
+      <c r="D74" s="74" t="s">
         <v>88</v>
       </c>
-      <c r="E74" s="70"/>
-      <c r="F74" s="71"/>
-      <c r="G74" s="72"/>
+      <c r="E74" s="74"/>
+      <c r="F74" s="75"/>
+      <c r="G74" s="76"/>
     </row>
     <row r="75" spans="1:7" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A75" s="76"/>
-      <c r="B75" s="70"/>
-      <c r="C75" s="70"/>
-      <c r="D75" s="70" t="s">
+      <c r="A75" s="80"/>
+      <c r="B75" s="74"/>
+      <c r="C75" s="74"/>
+      <c r="D75" s="74" t="s">
         <v>89</v>
       </c>
-      <c r="E75" s="70"/>
-      <c r="F75" s="71"/>
-      <c r="G75" s="72"/>
+      <c r="E75" s="74"/>
+      <c r="F75" s="75"/>
+      <c r="G75" s="76"/>
     </row>
   </sheetData>
   <mergeCells count="117">
@@ -6371,15 +6391,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="1" customFormat="1" ht="32.25" customHeight="1">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
       <c r="J1" s="2"/>
       <c r="L1" s="3"/>
       <c r="M1" s="4"/>
@@ -6388,15 +6408,15 @@
       <c r="P1" s="4"/>
     </row>
     <row r="2" spans="1:17" s="1" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
       <c r="J2" s="2"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
@@ -6409,10 +6429,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="5"/>
-      <c r="C3" s="45" t="s">
+      <c r="C3" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="45"/>
+      <c r="D3" s="54"/>
       <c r="E3" s="6"/>
       <c r="F3" s="5" t="s">
         <v>4</v>
@@ -6430,10 +6450,10 @@
         <v>5</v>
       </c>
       <c r="B4" s="5"/>
-      <c r="C4" s="45" t="s">
+      <c r="C4" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="45"/>
+      <c r="D4" s="54"/>
       <c r="E4" s="10"/>
       <c r="F4" s="11" t="s">
         <v>7</v>
@@ -6447,19 +6467,19 @@
       <c r="Q4" s="4"/>
     </row>
     <row r="5" spans="1:17" s="8" customFormat="1" ht="49.5" customHeight="1">
-      <c r="A5" s="60" t="s">
+      <c r="A5" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="46" t="s">
+      <c r="B5" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="48">
+      <c r="C5" s="63">
         <v>6</v>
       </c>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="50"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="64"/>
+      <c r="F5" s="64"/>
+      <c r="G5" s="65"/>
       <c r="H5" s="31"/>
       <c r="J5" s="12"/>
       <c r="K5" s="4"/>
@@ -6471,28 +6491,28 @@
       <c r="Q5" s="4"/>
     </row>
     <row r="6" spans="1:17" s="13" customFormat="1" ht="48" customHeight="1">
-      <c r="A6" s="61"/>
-      <c r="B6" s="47"/>
-      <c r="C6" s="62"/>
-      <c r="D6" s="63"/>
-      <c r="E6" s="63"/>
-      <c r="F6" s="63"/>
-      <c r="G6" s="64"/>
+      <c r="A6" s="60"/>
+      <c r="B6" s="62"/>
+      <c r="C6" s="66"/>
+      <c r="D6" s="67"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="67"/>
+      <c r="G6" s="68"/>
       <c r="I6" s="14"/>
       <c r="J6" s="14"/>
       <c r="K6" s="14"/>
       <c r="L6" s="14"/>
     </row>
     <row r="7" spans="1:17" s="8" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A7" s="54" t="s">
+      <c r="A7" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="59"/>
-      <c r="C7" s="59"/>
-      <c r="D7" s="59"/>
-      <c r="E7" s="59"/>
-      <c r="F7" s="59"/>
-      <c r="G7" s="55"/>
+      <c r="B7" s="52"/>
+      <c r="C7" s="52"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="52"/>
+      <c r="F7" s="52"/>
+      <c r="G7" s="50"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
@@ -6502,14 +6522,14 @@
       <c r="A8" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="54" t="s">
+      <c r="B8" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="55"/>
-      <c r="D8" s="56" t="s">
+      <c r="C8" s="50"/>
+      <c r="D8" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="56"/>
+      <c r="E8" s="51"/>
       <c r="F8" s="16" t="s">
         <v>14</v>
       </c>
@@ -6522,13 +6542,13 @@
       <c r="L8" s="4"/>
     </row>
     <row r="9" spans="1:17" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A9" s="101" t="s">
+      <c r="A9" s="105" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="104" t="s">
+      <c r="B9" s="108" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="105"/>
+      <c r="C9" s="109"/>
       <c r="D9" s="57" t="s">
         <v>18</v>
       </c>
@@ -6542,19 +6562,19 @@
       <c r="K9" s="4"/>
     </row>
     <row r="10" spans="1:17" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A10" s="102"/>
-      <c r="B10" s="95" t="s">
+      <c r="A10" s="106"/>
+      <c r="B10" s="99" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="96"/>
+      <c r="C10" s="100"/>
       <c r="D10" s="57" t="s">
         <v>21</v>
       </c>
       <c r="E10" s="58"/>
-      <c r="F10" s="74">
+      <c r="F10" s="78">
         <v>2</v>
       </c>
-      <c r="G10" s="114" t="s">
+      <c r="G10" s="120" t="s">
         <v>22</v>
       </c>
       <c r="K10" s="4"/>
@@ -6563,79 +6583,79 @@
       <c r="N10" s="4"/>
     </row>
     <row r="11" spans="1:17" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A11" s="102"/>
-      <c r="B11" s="97"/>
-      <c r="C11" s="98"/>
+      <c r="A11" s="106"/>
+      <c r="B11" s="101"/>
+      <c r="C11" s="102"/>
       <c r="D11" s="57" t="s">
         <v>23</v>
       </c>
       <c r="E11" s="58"/>
-      <c r="F11" s="94"/>
-      <c r="G11" s="115"/>
+      <c r="F11" s="98"/>
+      <c r="G11" s="121"/>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
       <c r="M11" s="4"/>
       <c r="N11" s="4"/>
     </row>
     <row r="12" spans="1:17" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A12" s="102"/>
-      <c r="B12" s="97"/>
-      <c r="C12" s="98"/>
+      <c r="A12" s="106"/>
+      <c r="B12" s="101"/>
+      <c r="C12" s="102"/>
       <c r="D12" s="57" t="s">
         <v>24</v>
       </c>
       <c r="E12" s="58"/>
-      <c r="F12" s="94"/>
-      <c r="G12" s="115"/>
+      <c r="F12" s="98"/>
+      <c r="G12" s="121"/>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
     </row>
     <row r="13" spans="1:17" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A13" s="102"/>
-      <c r="B13" s="97"/>
-      <c r="C13" s="98"/>
+      <c r="A13" s="106"/>
+      <c r="B13" s="101"/>
+      <c r="C13" s="102"/>
       <c r="D13" s="57" t="s">
         <v>25</v>
       </c>
       <c r="E13" s="58"/>
-      <c r="F13" s="94"/>
-      <c r="G13" s="115"/>
+      <c r="F13" s="98"/>
+      <c r="G13" s="121"/>
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
     </row>
     <row r="14" spans="1:17" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A14" s="102"/>
-      <c r="B14" s="99"/>
-      <c r="C14" s="100"/>
+      <c r="A14" s="106"/>
+      <c r="B14" s="103"/>
+      <c r="C14" s="104"/>
       <c r="D14" s="57" t="s">
         <v>26</v>
       </c>
       <c r="E14" s="58"/>
-      <c r="F14" s="75"/>
-      <c r="G14" s="115"/>
+      <c r="F14" s="79"/>
+      <c r="G14" s="121"/>
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
     </row>
     <row r="15" spans="1:17" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A15" s="102"/>
-      <c r="B15" s="88" t="s">
+      <c r="A15" s="106"/>
+      <c r="B15" s="92" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="89"/>
+      <c r="C15" s="93"/>
       <c r="D15" s="57" t="s">
         <v>28</v>
       </c>
       <c r="E15" s="58"/>
-      <c r="F15" s="74">
+      <c r="F15" s="78">
         <v>2</v>
       </c>
-      <c r="G15" s="115"/>
+      <c r="G15" s="121"/>
       <c r="H15" s="19"/>
       <c r="I15" s="19"/>
       <c r="J15" s="19"/>
@@ -6645,15 +6665,15 @@
       <c r="N15" s="4"/>
     </row>
     <row r="16" spans="1:17" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A16" s="102"/>
-      <c r="B16" s="92"/>
-      <c r="C16" s="93"/>
+      <c r="A16" s="106"/>
+      <c r="B16" s="96"/>
+      <c r="C16" s="97"/>
       <c r="D16" s="57" t="s">
         <v>29</v>
       </c>
       <c r="E16" s="58"/>
-      <c r="F16" s="94"/>
-      <c r="G16" s="115"/>
+      <c r="F16" s="98"/>
+      <c r="G16" s="121"/>
       <c r="H16" s="19"/>
       <c r="I16" s="19"/>
       <c r="J16" s="19"/>
@@ -6663,15 +6683,15 @@
       <c r="N16" s="4"/>
     </row>
     <row r="17" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A17" s="102"/>
-      <c r="B17" s="92"/>
-      <c r="C17" s="93"/>
+      <c r="A17" s="106"/>
+      <c r="B17" s="96"/>
+      <c r="C17" s="97"/>
       <c r="D17" s="57" t="s">
         <v>30</v>
       </c>
       <c r="E17" s="58"/>
-      <c r="F17" s="94"/>
-      <c r="G17" s="115"/>
+      <c r="F17" s="98"/>
+      <c r="G17" s="121"/>
       <c r="H17" s="19"/>
       <c r="I17" s="19"/>
       <c r="J17" s="19"/>
@@ -6681,15 +6701,15 @@
       <c r="N17" s="4"/>
     </row>
     <row r="18" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A18" s="102"/>
-      <c r="B18" s="92"/>
-      <c r="C18" s="93"/>
+      <c r="A18" s="106"/>
+      <c r="B18" s="96"/>
+      <c r="C18" s="97"/>
       <c r="D18" s="57" t="s">
         <v>31</v>
       </c>
       <c r="E18" s="58"/>
-      <c r="F18" s="94"/>
-      <c r="G18" s="115"/>
+      <c r="F18" s="98"/>
+      <c r="G18" s="121"/>
       <c r="H18" s="19"/>
       <c r="I18" s="19"/>
       <c r="J18" s="19"/>
@@ -6699,15 +6719,15 @@
       <c r="N18" s="4"/>
     </row>
     <row r="19" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A19" s="102"/>
-      <c r="B19" s="90"/>
-      <c r="C19" s="91"/>
+      <c r="A19" s="106"/>
+      <c r="B19" s="94"/>
+      <c r="C19" s="95"/>
       <c r="D19" s="57" t="s">
         <v>32</v>
       </c>
       <c r="E19" s="58"/>
-      <c r="F19" s="75"/>
-      <c r="G19" s="116"/>
+      <c r="F19" s="79"/>
+      <c r="G19" s="122"/>
       <c r="H19" s="19"/>
       <c r="I19" s="19"/>
       <c r="J19" s="19"/>
@@ -6717,19 +6737,19 @@
       <c r="N19" s="4"/>
     </row>
     <row r="20" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A20" s="102"/>
-      <c r="B20" s="88" t="s">
+      <c r="A20" s="106"/>
+      <c r="B20" s="92" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="89"/>
+      <c r="C20" s="93"/>
       <c r="D20" s="57" t="s">
         <v>34</v>
       </c>
       <c r="E20" s="58"/>
-      <c r="F20" s="74">
+      <c r="F20" s="78">
         <v>0</v>
       </c>
-      <c r="G20" s="114" t="s">
+      <c r="G20" s="120" t="s">
         <v>35</v>
       </c>
       <c r="K20" s="4"/>
@@ -6738,34 +6758,34 @@
       <c r="N20" s="4"/>
     </row>
     <row r="21" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A21" s="102"/>
-      <c r="B21" s="90"/>
-      <c r="C21" s="91"/>
+      <c r="A21" s="106"/>
+      <c r="B21" s="94"/>
+      <c r="C21" s="95"/>
       <c r="D21" s="57" t="s">
         <v>33</v>
       </c>
       <c r="E21" s="58"/>
-      <c r="F21" s="75"/>
-      <c r="G21" s="116"/>
+      <c r="F21" s="79"/>
+      <c r="G21" s="122"/>
       <c r="K21" s="4"/>
       <c r="L21" s="4"/>
       <c r="M21" s="4"/>
       <c r="N21" s="4"/>
     </row>
     <row r="22" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A22" s="102"/>
-      <c r="B22" s="95" t="s">
+      <c r="A22" s="106"/>
+      <c r="B22" s="99" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="96"/>
+      <c r="C22" s="100"/>
       <c r="D22" s="57" t="s">
         <v>37</v>
       </c>
       <c r="E22" s="58"/>
-      <c r="F22" s="74">
+      <c r="F22" s="78">
         <v>2</v>
       </c>
-      <c r="G22" s="65" t="s">
+      <c r="G22" s="69" t="s">
         <v>22</v>
       </c>
       <c r="K22" s="4"/>
@@ -6774,79 +6794,79 @@
       <c r="N22" s="4"/>
     </row>
     <row r="23" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A23" s="102"/>
-      <c r="B23" s="97"/>
-      <c r="C23" s="98"/>
+      <c r="A23" s="106"/>
+      <c r="B23" s="101"/>
+      <c r="C23" s="102"/>
       <c r="D23" s="57" t="s">
         <v>38</v>
       </c>
       <c r="E23" s="58"/>
-      <c r="F23" s="94"/>
-      <c r="G23" s="66"/>
+      <c r="F23" s="98"/>
+      <c r="G23" s="70"/>
       <c r="K23" s="4"/>
       <c r="L23" s="4"/>
       <c r="M23" s="4"/>
       <c r="N23" s="4"/>
     </row>
     <row r="24" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A24" s="102"/>
-      <c r="B24" s="97"/>
-      <c r="C24" s="98"/>
+      <c r="A24" s="106"/>
+      <c r="B24" s="101"/>
+      <c r="C24" s="102"/>
       <c r="D24" s="57" t="s">
         <v>39</v>
       </c>
       <c r="E24" s="58"/>
-      <c r="F24" s="94"/>
-      <c r="G24" s="66"/>
+      <c r="F24" s="98"/>
+      <c r="G24" s="70"/>
       <c r="K24" s="4"/>
       <c r="L24" s="4"/>
       <c r="M24" s="4"/>
       <c r="N24" s="4"/>
     </row>
     <row r="25" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A25" s="102"/>
-      <c r="B25" s="97"/>
-      <c r="C25" s="98"/>
+      <c r="A25" s="106"/>
+      <c r="B25" s="101"/>
+      <c r="C25" s="102"/>
       <c r="D25" s="57" t="s">
         <v>40</v>
       </c>
       <c r="E25" s="58"/>
-      <c r="F25" s="94"/>
-      <c r="G25" s="66"/>
+      <c r="F25" s="98"/>
+      <c r="G25" s="70"/>
       <c r="K25" s="4"/>
       <c r="L25" s="4"/>
       <c r="M25" s="4"/>
       <c r="N25" s="4"/>
     </row>
     <row r="26" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A26" s="102"/>
-      <c r="B26" s="99"/>
-      <c r="C26" s="100"/>
+      <c r="A26" s="106"/>
+      <c r="B26" s="103"/>
+      <c r="C26" s="104"/>
       <c r="D26" s="57" t="s">
         <v>41</v>
       </c>
       <c r="E26" s="58"/>
-      <c r="F26" s="75"/>
-      <c r="G26" s="66"/>
+      <c r="F26" s="79"/>
+      <c r="G26" s="70"/>
       <c r="K26" s="4"/>
       <c r="L26" s="4"/>
       <c r="M26" s="4"/>
       <c r="P26" s="4"/>
     </row>
     <row r="27" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A27" s="102"/>
-      <c r="B27" s="88" t="s">
+      <c r="A27" s="106"/>
+      <c r="B27" s="92" t="s">
         <v>42</v>
       </c>
-      <c r="C27" s="89"/>
+      <c r="C27" s="93"/>
       <c r="D27" s="57" t="s">
         <v>43</v>
       </c>
       <c r="E27" s="58"/>
-      <c r="F27" s="74">
+      <c r="F27" s="78">
         <v>2</v>
       </c>
-      <c r="G27" s="66"/>
+      <c r="G27" s="70"/>
       <c r="H27" s="19"/>
       <c r="I27" s="19"/>
       <c r="J27" s="19"/>
@@ -6856,15 +6876,15 @@
       <c r="N27" s="4"/>
     </row>
     <row r="28" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A28" s="102"/>
-      <c r="B28" s="92"/>
-      <c r="C28" s="93"/>
+      <c r="A28" s="106"/>
+      <c r="B28" s="96"/>
+      <c r="C28" s="97"/>
       <c r="D28" s="57" t="s">
         <v>44</v>
       </c>
       <c r="E28" s="58"/>
-      <c r="F28" s="94"/>
-      <c r="G28" s="66"/>
+      <c r="F28" s="98"/>
+      <c r="G28" s="70"/>
       <c r="H28" s="19"/>
       <c r="I28" s="19"/>
       <c r="J28" s="19"/>
@@ -6873,15 +6893,15 @@
       <c r="M28" s="20"/>
     </row>
     <row r="29" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A29" s="102"/>
-      <c r="B29" s="92"/>
-      <c r="C29" s="93"/>
+      <c r="A29" s="106"/>
+      <c r="B29" s="96"/>
+      <c r="C29" s="97"/>
       <c r="D29" s="57" t="s">
         <v>45</v>
       </c>
       <c r="E29" s="58"/>
-      <c r="F29" s="94"/>
-      <c r="G29" s="66"/>
+      <c r="F29" s="98"/>
+      <c r="G29" s="70"/>
       <c r="H29" s="19"/>
       <c r="I29" s="19"/>
       <c r="J29" s="19"/>
@@ -6890,15 +6910,15 @@
       <c r="M29" s="20"/>
     </row>
     <row r="30" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A30" s="102"/>
-      <c r="B30" s="92"/>
-      <c r="C30" s="93"/>
+      <c r="A30" s="106"/>
+      <c r="B30" s="96"/>
+      <c r="C30" s="97"/>
       <c r="D30" s="57" t="s">
         <v>46</v>
       </c>
       <c r="E30" s="58"/>
-      <c r="F30" s="94"/>
-      <c r="G30" s="66"/>
+      <c r="F30" s="98"/>
+      <c r="G30" s="70"/>
       <c r="H30" s="19"/>
       <c r="I30" s="19"/>
       <c r="J30" s="19"/>
@@ -6907,15 +6927,15 @@
       <c r="M30" s="20"/>
     </row>
     <row r="31" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A31" s="102"/>
-      <c r="B31" s="90"/>
-      <c r="C31" s="91"/>
+      <c r="A31" s="106"/>
+      <c r="B31" s="94"/>
+      <c r="C31" s="95"/>
       <c r="D31" s="57" t="s">
         <v>47</v>
       </c>
       <c r="E31" s="58"/>
-      <c r="F31" s="75"/>
-      <c r="G31" s="66"/>
+      <c r="F31" s="79"/>
+      <c r="G31" s="70"/>
       <c r="H31" s="19"/>
       <c r="I31" s="19"/>
       <c r="J31" s="19"/>
@@ -6924,19 +6944,19 @@
       <c r="M31" s="20"/>
     </row>
     <row r="32" spans="1:16" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A32" s="102"/>
-      <c r="B32" s="88" t="s">
+      <c r="A32" s="106"/>
+      <c r="B32" s="92" t="s">
         <v>48</v>
       </c>
-      <c r="C32" s="89"/>
+      <c r="C32" s="93"/>
       <c r="D32" s="57" t="s">
         <v>49</v>
       </c>
       <c r="E32" s="58"/>
-      <c r="F32" s="74">
+      <c r="F32" s="78">
         <v>2</v>
       </c>
-      <c r="G32" s="66" t="s">
+      <c r="G32" s="70" t="s">
         <v>50</v>
       </c>
       <c r="H32" s="19"/>
@@ -6948,15 +6968,15 @@
       <c r="N32" s="4"/>
     </row>
     <row r="33" spans="1:15" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A33" s="102"/>
-      <c r="B33" s="92"/>
-      <c r="C33" s="93"/>
+      <c r="A33" s="106"/>
+      <c r="B33" s="96"/>
+      <c r="C33" s="97"/>
       <c r="D33" s="57" t="s">
         <v>51</v>
       </c>
       <c r="E33" s="58"/>
-      <c r="F33" s="94"/>
-      <c r="G33" s="66"/>
+      <c r="F33" s="98"/>
+      <c r="G33" s="70"/>
       <c r="H33" s="19"/>
       <c r="I33" s="19"/>
       <c r="J33" s="19"/>
@@ -6966,15 +6986,15 @@
       <c r="N33" s="4"/>
     </row>
     <row r="34" spans="1:15" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A34" s="102"/>
-      <c r="B34" s="92"/>
-      <c r="C34" s="93"/>
+      <c r="A34" s="106"/>
+      <c r="B34" s="96"/>
+      <c r="C34" s="97"/>
       <c r="D34" s="57" t="s">
         <v>52</v>
       </c>
       <c r="E34" s="58"/>
-      <c r="F34" s="94"/>
-      <c r="G34" s="66"/>
+      <c r="F34" s="98"/>
+      <c r="G34" s="70"/>
       <c r="H34" s="19"/>
       <c r="I34" s="19"/>
       <c r="J34" s="19"/>
@@ -6984,15 +7004,15 @@
       <c r="N34" s="4"/>
     </row>
     <row r="35" spans="1:15" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A35" s="102"/>
-      <c r="B35" s="92"/>
-      <c r="C35" s="93"/>
+      <c r="A35" s="106"/>
+      <c r="B35" s="96"/>
+      <c r="C35" s="97"/>
       <c r="D35" s="57" t="s">
         <v>53</v>
       </c>
       <c r="E35" s="58"/>
-      <c r="F35" s="94"/>
-      <c r="G35" s="66"/>
+      <c r="F35" s="98"/>
+      <c r="G35" s="70"/>
       <c r="H35" s="19"/>
       <c r="I35" s="19"/>
       <c r="J35" s="19"/>
@@ -7002,15 +7022,15 @@
       <c r="N35" s="4"/>
     </row>
     <row r="36" spans="1:15" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A36" s="102"/>
-      <c r="B36" s="90"/>
-      <c r="C36" s="91"/>
+      <c r="A36" s="106"/>
+      <c r="B36" s="94"/>
+      <c r="C36" s="95"/>
       <c r="D36" s="57" t="s">
         <v>54</v>
       </c>
       <c r="E36" s="58"/>
-      <c r="F36" s="75"/>
-      <c r="G36" s="66"/>
+      <c r="F36" s="79"/>
+      <c r="G36" s="70"/>
       <c r="H36" s="19"/>
       <c r="I36" s="19"/>
       <c r="J36" s="19"/>
@@ -7020,98 +7040,98 @@
       <c r="N36" s="4"/>
     </row>
     <row r="37" spans="1:15" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A37" s="102"/>
-      <c r="B37" s="88" t="s">
+      <c r="A37" s="106"/>
+      <c r="B37" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="C37" s="89"/>
+      <c r="C37" s="93"/>
       <c r="D37" s="57" t="s">
         <v>56</v>
       </c>
       <c r="E37" s="58"/>
-      <c r="F37" s="74">
+      <c r="F37" s="78">
         <v>2</v>
       </c>
-      <c r="G37" s="66"/>
+      <c r="G37" s="70"/>
       <c r="K37" s="4"/>
       <c r="L37" s="4"/>
       <c r="M37" s="4"/>
       <c r="N37" s="4"/>
     </row>
     <row r="38" spans="1:15" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A38" s="102"/>
-      <c r="B38" s="92"/>
-      <c r="C38" s="93"/>
+      <c r="A38" s="106"/>
+      <c r="B38" s="96"/>
+      <c r="C38" s="97"/>
       <c r="D38" s="57" t="s">
         <v>23</v>
       </c>
       <c r="E38" s="58"/>
-      <c r="F38" s="94"/>
-      <c r="G38" s="66"/>
+      <c r="F38" s="98"/>
+      <c r="G38" s="70"/>
       <c r="K38" s="4"/>
       <c r="L38" s="4"/>
       <c r="M38" s="4"/>
       <c r="N38" s="4"/>
     </row>
     <row r="39" spans="1:15" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A39" s="102"/>
-      <c r="B39" s="92"/>
-      <c r="C39" s="93"/>
+      <c r="A39" s="106"/>
+      <c r="B39" s="96"/>
+      <c r="C39" s="97"/>
       <c r="D39" s="57" t="s">
         <v>41</v>
       </c>
       <c r="E39" s="58"/>
-      <c r="F39" s="94"/>
-      <c r="G39" s="66"/>
+      <c r="F39" s="98"/>
+      <c r="G39" s="70"/>
       <c r="K39" s="4"/>
       <c r="L39" s="4"/>
       <c r="M39" s="4"/>
       <c r="N39" s="4"/>
     </row>
     <row r="40" spans="1:15" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A40" s="102"/>
-      <c r="B40" s="92"/>
-      <c r="C40" s="93"/>
+      <c r="A40" s="106"/>
+      <c r="B40" s="96"/>
+      <c r="C40" s="97"/>
       <c r="D40" s="57" t="s">
         <v>57</v>
       </c>
       <c r="E40" s="58"/>
-      <c r="F40" s="94"/>
-      <c r="G40" s="66"/>
+      <c r="F40" s="98"/>
+      <c r="G40" s="70"/>
       <c r="K40" s="21"/>
       <c r="L40" s="21"/>
       <c r="M40" s="4"/>
       <c r="N40" s="4"/>
     </row>
     <row r="41" spans="1:15" s="8" customFormat="1" ht="22" customHeight="1">
-      <c r="A41" s="102"/>
-      <c r="B41" s="90"/>
-      <c r="C41" s="91"/>
+      <c r="A41" s="106"/>
+      <c r="B41" s="94"/>
+      <c r="C41" s="95"/>
       <c r="D41" s="57" t="s">
         <v>58</v>
       </c>
       <c r="E41" s="58"/>
-      <c r="F41" s="75"/>
-      <c r="G41" s="67"/>
+      <c r="F41" s="79"/>
+      <c r="G41" s="71"/>
       <c r="K41" s="4"/>
       <c r="L41" s="4"/>
       <c r="M41" s="4"/>
       <c r="N41" s="4"/>
     </row>
     <row r="42" spans="1:15" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A42" s="102"/>
-      <c r="B42" s="88" t="s">
+      <c r="A42" s="106"/>
+      <c r="B42" s="92" t="s">
         <v>59</v>
       </c>
-      <c r="C42" s="89"/>
+      <c r="C42" s="93"/>
       <c r="D42" s="57" t="s">
         <v>60</v>
       </c>
       <c r="E42" s="58"/>
-      <c r="F42" s="74">
+      <c r="F42" s="78">
         <v>0</v>
       </c>
-      <c r="G42" s="65" t="s">
+      <c r="G42" s="69" t="s">
         <v>35</v>
       </c>
       <c r="K42" s="21"/>
@@ -7121,34 +7141,34 @@
       <c r="O42" s="8"/>
     </row>
     <row r="43" spans="1:15" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A43" s="102"/>
-      <c r="B43" s="90"/>
-      <c r="C43" s="91"/>
+      <c r="A43" s="106"/>
+      <c r="B43" s="94"/>
+      <c r="C43" s="95"/>
       <c r="D43" s="57" t="s">
         <v>61</v>
       </c>
       <c r="E43" s="58"/>
-      <c r="F43" s="75"/>
-      <c r="G43" s="67"/>
+      <c r="F43" s="79"/>
+      <c r="G43" s="71"/>
       <c r="K43" s="21"/>
       <c r="L43" s="21"/>
       <c r="M43" s="21"/>
       <c r="N43" s="21"/>
     </row>
     <row r="44" spans="1:15" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A44" s="102"/>
-      <c r="B44" s="88" t="s">
+      <c r="A44" s="106"/>
+      <c r="B44" s="92" t="s">
         <v>62</v>
       </c>
-      <c r="C44" s="89"/>
+      <c r="C44" s="93"/>
       <c r="D44" s="57" t="s">
         <v>63</v>
       </c>
       <c r="E44" s="58"/>
-      <c r="F44" s="74">
+      <c r="F44" s="78">
         <v>0</v>
       </c>
-      <c r="G44" s="65" t="s">
+      <c r="G44" s="69" t="s">
         <v>22</v>
       </c>
       <c r="H44" s="8"/>
@@ -7160,15 +7180,15 @@
       <c r="N44" s="21"/>
     </row>
     <row r="45" spans="1:15" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A45" s="102"/>
-      <c r="B45" s="90"/>
-      <c r="C45" s="91"/>
+      <c r="A45" s="106"/>
+      <c r="B45" s="94"/>
+      <c r="C45" s="95"/>
       <c r="D45" s="57" t="s">
         <v>64</v>
       </c>
       <c r="E45" s="58"/>
-      <c r="F45" s="75"/>
-      <c r="G45" s="66"/>
+      <c r="F45" s="79"/>
+      <c r="G45" s="70"/>
       <c r="H45" s="23"/>
       <c r="I45" s="23"/>
       <c r="J45" s="23"/>
@@ -7178,111 +7198,111 @@
       <c r="N45" s="21"/>
     </row>
     <row r="46" spans="1:15" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A46" s="102"/>
-      <c r="B46" s="88" t="s">
+      <c r="A46" s="106"/>
+      <c r="B46" s="92" t="s">
         <v>65</v>
       </c>
-      <c r="C46" s="89"/>
+      <c r="C46" s="93"/>
       <c r="D46" s="57" t="s">
         <v>66</v>
       </c>
       <c r="E46" s="58"/>
-      <c r="F46" s="74">
+      <c r="F46" s="78">
         <v>0</v>
       </c>
-      <c r="G46" s="66"/>
+      <c r="G46" s="70"/>
       <c r="K46" s="21"/>
       <c r="L46" s="21"/>
       <c r="M46" s="21"/>
       <c r="N46" s="21"/>
     </row>
     <row r="47" spans="1:15" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A47" s="102"/>
-      <c r="B47" s="92"/>
-      <c r="C47" s="93"/>
+      <c r="A47" s="106"/>
+      <c r="B47" s="96"/>
+      <c r="C47" s="97"/>
       <c r="D47" s="57" t="s">
         <v>67</v>
       </c>
       <c r="E47" s="58"/>
-      <c r="F47" s="94"/>
-      <c r="G47" s="66"/>
+      <c r="F47" s="98"/>
+      <c r="G47" s="70"/>
       <c r="K47" s="21"/>
       <c r="L47" s="21"/>
       <c r="M47" s="21"/>
       <c r="N47" s="21"/>
     </row>
     <row r="48" spans="1:15" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A48" s="102"/>
-      <c r="B48" s="92"/>
-      <c r="C48" s="93"/>
+      <c r="A48" s="106"/>
+      <c r="B48" s="96"/>
+      <c r="C48" s="97"/>
       <c r="D48" s="57" t="s">
         <v>68</v>
       </c>
       <c r="E48" s="58"/>
-      <c r="F48" s="94"/>
-      <c r="G48" s="66"/>
+      <c r="F48" s="98"/>
+      <c r="G48" s="70"/>
       <c r="K48" s="21"/>
       <c r="L48" s="21"/>
       <c r="M48" s="21"/>
       <c r="N48" s="21"/>
     </row>
     <row r="49" spans="1:16" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A49" s="102"/>
-      <c r="B49" s="92"/>
-      <c r="C49" s="93"/>
+      <c r="A49" s="106"/>
+      <c r="B49" s="96"/>
+      <c r="C49" s="97"/>
       <c r="D49" s="57" t="s">
         <v>69</v>
       </c>
       <c r="E49" s="58"/>
-      <c r="F49" s="94"/>
-      <c r="G49" s="66"/>
+      <c r="F49" s="98"/>
+      <c r="G49" s="70"/>
       <c r="K49" s="21"/>
       <c r="L49" s="21"/>
       <c r="M49" s="21"/>
       <c r="N49" s="21"/>
     </row>
     <row r="50" spans="1:16" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A50" s="102"/>
-      <c r="B50" s="92"/>
-      <c r="C50" s="93"/>
+      <c r="A50" s="106"/>
+      <c r="B50" s="96"/>
+      <c r="C50" s="97"/>
       <c r="D50" s="57" t="s">
         <v>70</v>
       </c>
       <c r="E50" s="58"/>
-      <c r="F50" s="94"/>
-      <c r="G50" s="66"/>
+      <c r="F50" s="98"/>
+      <c r="G50" s="70"/>
       <c r="K50" s="21"/>
       <c r="L50" s="21"/>
       <c r="M50" s="21"/>
       <c r="N50" s="21"/>
     </row>
     <row r="51" spans="1:16" s="22" customFormat="1" ht="22" customHeight="1">
-      <c r="A51" s="103"/>
-      <c r="B51" s="90"/>
-      <c r="C51" s="91"/>
+      <c r="A51" s="107"/>
+      <c r="B51" s="94"/>
+      <c r="C51" s="95"/>
       <c r="D51" s="57" t="s">
         <v>71</v>
       </c>
       <c r="E51" s="58"/>
-      <c r="F51" s="75"/>
-      <c r="G51" s="67"/>
+      <c r="F51" s="79"/>
+      <c r="G51" s="71"/>
       <c r="K51" s="21"/>
       <c r="L51" s="21"/>
       <c r="M51" s="21"/>
       <c r="N51" s="21"/>
     </row>
     <row r="52" spans="1:16" s="8" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A52" s="76" t="s">
+      <c r="A52" s="80" t="s">
         <v>72</v>
       </c>
-      <c r="B52" s="77" t="s">
+      <c r="B52" s="81" t="s">
         <v>73</v>
       </c>
-      <c r="C52" s="77"/>
-      <c r="D52" s="77" t="s">
+      <c r="C52" s="81"/>
+      <c r="D52" s="81" t="s">
         <v>74</v>
       </c>
-      <c r="E52" s="77"/>
+      <c r="E52" s="81"/>
       <c r="F52" s="17">
         <v>0</v>
       </c>
@@ -7294,15 +7314,15 @@
       <c r="M52" s="20"/>
     </row>
     <row r="53" spans="1:16" s="8" customFormat="1" ht="95.25" customHeight="1">
-      <c r="A53" s="76"/>
-      <c r="B53" s="78" t="s">
+      <c r="A53" s="80"/>
+      <c r="B53" s="82" t="s">
         <v>76</v>
       </c>
-      <c r="C53" s="78"/>
-      <c r="D53" s="72" t="s">
+      <c r="C53" s="82"/>
+      <c r="D53" s="76" t="s">
         <v>77</v>
       </c>
-      <c r="E53" s="72"/>
+      <c r="E53" s="76"/>
       <c r="F53" s="26">
         <v>0</v>
       </c>
@@ -7314,19 +7334,19 @@
       <c r="M53" s="20"/>
     </row>
     <row r="54" spans="1:16" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A54" s="76"/>
-      <c r="B54" s="79" t="s">
+      <c r="A54" s="80"/>
+      <c r="B54" s="83" t="s">
         <v>78</v>
       </c>
-      <c r="C54" s="80"/>
-      <c r="D54" s="68" t="s">
+      <c r="C54" s="84"/>
+      <c r="D54" s="72" t="s">
         <v>79</v>
       </c>
-      <c r="E54" s="69"/>
-      <c r="F54" s="85">
+      <c r="E54" s="73"/>
+      <c r="F54" s="89">
         <v>0</v>
       </c>
-      <c r="G54" s="65" t="s">
+      <c r="G54" s="69" t="s">
         <v>80</v>
       </c>
       <c r="K54" s="4"/>
@@ -7335,30 +7355,30 @@
       <c r="N54" s="4"/>
     </row>
     <row r="55" spans="1:16" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A55" s="76"/>
-      <c r="B55" s="81"/>
-      <c r="C55" s="82"/>
-      <c r="D55" s="68" t="s">
+      <c r="A55" s="80"/>
+      <c r="B55" s="85"/>
+      <c r="C55" s="86"/>
+      <c r="D55" s="72" t="s">
         <v>81</v>
       </c>
-      <c r="E55" s="69"/>
-      <c r="F55" s="86"/>
-      <c r="G55" s="66"/>
+      <c r="E55" s="73"/>
+      <c r="F55" s="90"/>
+      <c r="G55" s="70"/>
       <c r="K55" s="4"/>
       <c r="L55" s="4"/>
       <c r="M55" s="4"/>
       <c r="N55" s="4"/>
     </row>
     <row r="56" spans="1:16" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A56" s="76"/>
-      <c r="B56" s="81"/>
-      <c r="C56" s="82"/>
-      <c r="D56" s="68" t="s">
+      <c r="A56" s="80"/>
+      <c r="B56" s="85"/>
+      <c r="C56" s="86"/>
+      <c r="D56" s="72" t="s">
         <v>82</v>
       </c>
-      <c r="E56" s="69"/>
-      <c r="F56" s="86"/>
-      <c r="G56" s="66"/>
+      <c r="E56" s="73"/>
+      <c r="F56" s="90"/>
+      <c r="G56" s="70"/>
       <c r="J56" s="4"/>
       <c r="K56" s="4"/>
       <c r="L56" s="4"/>
@@ -7366,15 +7386,15 @@
       <c r="N56" s="4"/>
     </row>
     <row r="57" spans="1:16" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A57" s="76"/>
-      <c r="B57" s="83"/>
-      <c r="C57" s="84"/>
-      <c r="D57" s="68" t="s">
+      <c r="A57" s="80"/>
+      <c r="B57" s="87"/>
+      <c r="C57" s="88"/>
+      <c r="D57" s="72" t="s">
         <v>83</v>
       </c>
-      <c r="E57" s="69"/>
-      <c r="F57" s="87"/>
-      <c r="G57" s="67"/>
+      <c r="E57" s="73"/>
+      <c r="F57" s="91"/>
+      <c r="G57" s="71"/>
       <c r="H57" s="1"/>
       <c r="I57" s="1"/>
       <c r="J57" s="3"/>
@@ -7384,19 +7404,19 @@
       <c r="N57" s="3"/>
     </row>
     <row r="58" spans="1:16" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A58" s="76"/>
-      <c r="B58" s="70" t="s">
+      <c r="A58" s="80"/>
+      <c r="B58" s="74" t="s">
         <v>84</v>
       </c>
-      <c r="C58" s="70"/>
-      <c r="D58" s="70" t="s">
+      <c r="C58" s="74"/>
+      <c r="D58" s="74" t="s">
         <v>85</v>
       </c>
-      <c r="E58" s="70"/>
-      <c r="F58" s="71">
+      <c r="E58" s="74"/>
+      <c r="F58" s="75">
         <v>0</v>
       </c>
-      <c r="G58" s="72" t="s">
+      <c r="G58" s="76" t="s">
         <v>86</v>
       </c>
       <c r="K58" s="4"/>
@@ -7405,44 +7425,44 @@
       <c r="N58" s="4"/>
     </row>
     <row r="59" spans="1:16" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A59" s="76"/>
-      <c r="B59" s="70"/>
-      <c r="C59" s="70"/>
-      <c r="D59" s="73" t="s">
+      <c r="A59" s="80"/>
+      <c r="B59" s="74"/>
+      <c r="C59" s="74"/>
+      <c r="D59" s="77" t="s">
         <v>87</v>
       </c>
-      <c r="E59" s="73"/>
-      <c r="F59" s="71"/>
-      <c r="G59" s="72"/>
+      <c r="E59" s="77"/>
+      <c r="F59" s="75"/>
+      <c r="G59" s="76"/>
       <c r="K59" s="4"/>
       <c r="L59" s="4"/>
       <c r="M59" s="4"/>
       <c r="N59" s="4"/>
     </row>
     <row r="60" spans="1:16" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A60" s="76"/>
-      <c r="B60" s="70"/>
-      <c r="C60" s="70"/>
-      <c r="D60" s="70" t="s">
+      <c r="A60" s="80"/>
+      <c r="B60" s="74"/>
+      <c r="C60" s="74"/>
+      <c r="D60" s="74" t="s">
         <v>88</v>
       </c>
-      <c r="E60" s="70"/>
-      <c r="F60" s="71"/>
-      <c r="G60" s="72"/>
+      <c r="E60" s="74"/>
+      <c r="F60" s="75"/>
+      <c r="G60" s="76"/>
       <c r="K60" s="4"/>
       <c r="L60" s="4"/>
       <c r="M60" s="4"/>
     </row>
     <row r="61" spans="1:16" s="8" customFormat="1" ht="25" customHeight="1">
-      <c r="A61" s="76"/>
-      <c r="B61" s="70"/>
-      <c r="C61" s="70"/>
-      <c r="D61" s="70" t="s">
+      <c r="A61" s="80"/>
+      <c r="B61" s="74"/>
+      <c r="C61" s="74"/>
+      <c r="D61" s="74" t="s">
         <v>89</v>
       </c>
-      <c r="E61" s="70"/>
-      <c r="F61" s="71"/>
-      <c r="G61" s="72"/>
+      <c r="E61" s="74"/>
+      <c r="F61" s="75"/>
+      <c r="G61" s="76"/>
       <c r="K61" s="4"/>
       <c r="L61" s="4"/>
       <c r="M61" s="4"/>

</xml_diff>